<commit_message>
Added functionality of send PID parameters (delays and setpoint).
</commit_message>
<xml_diff>
--- a/Resources/DataPacket/Commands.xlsx
+++ b/Resources/DataPacket/Commands.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavi\Documents\Embed\STM32\Projects\CurrentController\Resources\DataPacket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08444A5F-FFD8-4203-8826-A23C9A0F4744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4C1911-28C4-4589-BE8A-9636A922106E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Packet" sheetId="4" r:id="rId1"/>
@@ -213,18 +213,6 @@
     <t>0x17</t>
   </si>
   <si>
-    <t>0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00</t>
-  </si>
-  <si>
-    <t>0xAA 0x55 0x17 0x0C 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0xF3</t>
-  </si>
-  <si>
-    <t>0x0C</t>
-  </si>
-  <si>
-    <t>0xF3</t>
-  </si>
-  <si>
     <t>Sets the value of kp: [-128:127] = [0x00:0xFF]</t>
   </si>
   <si>
@@ -316,6 +304,18 @@
   </si>
   <si>
     <t>Sets the value of sampling delay: [0-65535] = [0x0000:0xFFFF]</t>
+  </si>
+  <si>
+    <t>0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x17 0x08 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x8A</t>
+  </si>
+  <si>
+    <t>0x08</t>
+  </si>
+  <si>
+    <t>0x8A</t>
   </si>
 </sst>
 </file>
@@ -40971,19 +40971,19 @@
   </sheetPr>
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="97.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -41054,7 +41054,7 @@
         <v>26</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>24</v>
@@ -41089,7 +41089,7 @@
         <v>26</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>24</v>
@@ -41124,7 +41124,7 @@
         <v>26</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>24</v>
@@ -41299,18 +41299,18 @@
         <v>26</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>14</v>
@@ -41322,19 +41322,19 @@
         <v>54</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>27</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>24</v>
@@ -41345,7 +41345,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>14</v>
@@ -41354,22 +41354,22 @@
         <v>15</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>26</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>24</v>
@@ -41380,7 +41380,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>14</v>
@@ -41389,22 +41389,22 @@
         <v>15</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>26</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>24</v>
@@ -41415,7 +41415,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>14</v>
@@ -41427,19 +41427,19 @@
         <v>19</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>26</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>24</v>
@@ -41450,7 +41450,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>14</v>
@@ -41459,22 +41459,22 @@
         <v>15</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>27</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="K14" s="5" t="s">
         <v>24</v>
@@ -41485,7 +41485,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>14</v>
@@ -41494,7 +41494,7 @@
         <v>15</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>22</v>
@@ -41503,13 +41503,13 @@
         <v>17</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>26</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K15" s="5" t="s">
         <v>18</v>
@@ -41520,7 +41520,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>14</v>
@@ -41529,7 +41529,7 @@
         <v>15</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>22</v>
@@ -41538,13 +41538,13 @@
         <v>22</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>26</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="K16" s="5" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Added functionality of receive PID parameters from computer.
</commit_message>
<xml_diff>
--- a/Resources/DataPacket/Commands.xlsx
+++ b/Resources/DataPacket/Commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavi\Documents\Embed\STM32\Projects\CurrentController\Resources\DataPacket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4C1911-28C4-4589-BE8A-9636A922106E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76873897-D925-4F4F-911C-D62D31B04372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -213,15 +213,6 @@
     <t>0x17</t>
   </si>
   <si>
-    <t>Sets the value of kp: [-128:127] = [0x00:0xFF]</t>
-  </si>
-  <si>
-    <t>Sets the value of ki: [-128:127] = [0x00:0xFF]</t>
-  </si>
-  <si>
-    <t>Sets the value of kd: [-128:127] = [0x00:0xFF]</t>
-  </si>
-  <si>
     <t>0x18</t>
   </si>
   <si>
@@ -235,9 +226,6 @@
   </si>
   <si>
     <t>0xDC</t>
-  </si>
-  <si>
-    <t>Sets the value of delay PID: [0-65535] = [0x0000:0xFFFF]</t>
   </si>
   <si>
     <t>0x19</t>
@@ -270,19 +258,7 @@
     <t>0xCE</t>
   </si>
   <si>
-    <t>Sets the value of Setpoint (electrical current in uA): [-2,147,483,648:2,147,483,647] = [0x00000000:0xFFFFFFFF]</t>
-  </si>
-  <si>
     <t>0x22</t>
-  </si>
-  <si>
-    <t>Sends the current process variable value (electrical current in uA): [-2,147,483,648:2,147,483,647] = [0x00000000:0xFFFFFFFF]</t>
-  </si>
-  <si>
-    <t>Disables the send of the current process variable value (electrical current in uA) from microcontroller to PC at each 50ms</t>
-  </si>
-  <si>
-    <t>Enables the send of the current process variable value (electrical current in uA) from microcontroller to PC at each 50ms</t>
   </si>
   <si>
     <t>0xAA 0x55 0x22 0x01 0x00 0x1C</t>
@@ -303,9 +279,6 @@
     <t>Sends the current sampling delay, delay PID, Setpoint values</t>
   </si>
   <si>
-    <t>Sets the value of sampling delay: [0-65535] = [0x0000:0xFFFF]</t>
-  </si>
-  <si>
     <t>0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00</t>
   </si>
   <si>
@@ -316,6 +289,33 @@
   </si>
   <si>
     <t>0x8A</t>
+  </si>
+  <si>
+    <t>Disables the send of the current process variable value (electrical current in uA) from microcontroller to PC at each 100ms</t>
+  </si>
+  <si>
+    <t>Enables the send of the current process variable value (electrical current in uA) from microcontroller to PC at each 100ms</t>
+  </si>
+  <si>
+    <t>Sets the value of sampling delay: [0 : 65535] = [0x0000 : 0xFFFF]</t>
+  </si>
+  <si>
+    <t>Sets the value of delay PID: [0 : 65535] = [0x0000 : 0xFFFF]</t>
+  </si>
+  <si>
+    <t>Sets the value of Setpoint (electrical current in uA): [0 : 4294967295] = [0x00000000 : 0xFFFFFFFF]</t>
+  </si>
+  <si>
+    <t>Sets the value of kp: [0 : 255] = [0x00 : 0xFF]</t>
+  </si>
+  <si>
+    <t>Sets the value of ki: [0 : 255] = [0x00 : 0xFF]</t>
+  </si>
+  <si>
+    <t>Sets the value of kd: [0 : 255] = [0x00 : 0xFF]</t>
+  </si>
+  <si>
+    <t>Sends the current process variable value (electrical current in uA): [0 : 4294967295] = [0x00000000 : 0xFFFFFFFF]</t>
   </si>
 </sst>
 </file>
@@ -360,12 +360,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -475,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -528,6 +534,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -40966,13 +40980,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B11DB8B0-5B17-4A82-8032-D4706BCA4450}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41025,178 +41039,178 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+    <row r="2" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>55</v>
+      <c r="J2" s="18" t="s">
+        <v>86</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+    <row r="3" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>56</v>
+      <c r="J3" s="18" t="s">
+        <v>87</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+    <row r="4" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="5" t="s">
-        <v>57</v>
+      <c r="J4" s="18" t="s">
+        <v>88</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+    <row r="5" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+    <row r="6" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="18" t="s">
         <v>24</v>
       </c>
     </row>
@@ -41270,294 +41284,288 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+    <row r="9" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="18">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18">
+        <v>9</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="18">
+        <v>10</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K11" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18">
+        <v>11</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="K12" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="18">
+        <v>12</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="K13" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="20">
+        <v>13</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="K14" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18">
+        <v>14</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="K15" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>9</v>
+    <row r="16" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18">
+        <v>15</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>87</v>
+      <c r="B16" s="18" t="s">
+        <v>73</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C16" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D16" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>54</v>
+      <c r="E16" s="18" t="s">
+        <v>70</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>88</v>
+      <c r="F16" s="18" t="s">
+        <v>22</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>86</v>
+      <c r="G16" s="18" t="s">
+        <v>22</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>89</v>
+      <c r="H16" s="18" t="s">
+        <v>74</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>10</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I11" s="5" t="s">
+      <c r="I16" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="5" t="s">
-        <v>85</v>
+      <c r="J16" s="18" t="s">
+        <v>82</v>
       </c>
-      <c r="K11" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>11</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>14</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="K15" s="5" t="s">
+      <c r="K16" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>15</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:K16" xr:uid="{B11DB8B0-5B17-4A82-8032-D4706BCA4450}">
-    <filterColumn colId="8">
-      <filters>
-        <filter val="From PC to Microcontroller"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K16" xr:uid="{B11DB8B0-5B17-4A82-8032-D4706BCA4450}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup scale="39" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added functionality of start and stop PID controller.
</commit_message>
<xml_diff>
--- a/Resources/DataPacket/Commands.xlsx
+++ b/Resources/DataPacket/Commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavi\Documents\Embed\STM32\Projects\CurrentController\Resources\DataPacket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76873897-D925-4F4F-911C-D62D31B04372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6958DE-587E-458A-BFDD-A451A69D401B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -481,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -504,6 +504,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -534,14 +538,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -844,14 +840,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -1416,13 +1412,13 @@
       <c r="AG6" s="3"/>
     </row>
     <row r="7" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -1453,11 +1449,11 @@
       <c r="AG7" s="3"/>
     </row>
     <row r="8" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1488,11 +1484,11 @@
       <c r="AG8" s="3"/>
     </row>
     <row r="9" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="15"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1523,11 +1519,11 @@
       <c r="AG9" s="3"/>
     </row>
     <row r="10" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -1558,11 +1554,11 @@
       <c r="AG10" s="3"/>
     </row>
     <row r="11" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="15"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -1593,11 +1589,11 @@
       <c r="AG11" s="3"/>
     </row>
     <row r="12" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="15"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -1628,11 +1624,11 @@
       <c r="AG12" s="3"/>
     </row>
     <row r="13" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="15"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -1663,11 +1659,11 @@
       <c r="AG13" s="3"/>
     </row>
     <row r="14" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="15"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1698,11 +1694,11 @@
       <c r="AG14" s="3"/>
     </row>
     <row r="15" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="13"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="15"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1733,11 +1729,11 @@
       <c r="AG15" s="3"/>
     </row>
     <row r="16" spans="1:369" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="16"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="18"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -40986,7 +40982,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41039,528 +41035,528 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18">
+    <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18">
+    <row r="3" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="K3" s="18" t="s">
+      <c r="K3" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18">
+    <row r="4" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="I4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="K4" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18">
+    <row r="5" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="J5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="K5" s="18" t="s">
+      <c r="K5" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18">
+    <row r="6" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="J6" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="K6" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+    <row r="7" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+    <row r="8" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
+    <row r="9" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
         <v>8</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="I9" s="18" t="s">
+      <c r="I9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="J9" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="K9" s="18" t="s">
+      <c r="K9" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18">
+    <row r="10" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="I10" s="18" t="s">
+      <c r="I10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="18" t="s">
+      <c r="J10" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="K10" s="18" t="s">
+      <c r="K10" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18">
+    <row r="11" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
         <v>10</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="18" t="s">
+      <c r="I11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="18" t="s">
+      <c r="J11" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="K11" s="18" t="s">
+      <c r="K11" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
+    <row r="12" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
         <v>11</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="I12" s="18" t="s">
+      <c r="I12" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="18" t="s">
+      <c r="J12" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="K12" s="18" t="s">
+      <c r="K12" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18">
+    <row r="13" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
         <v>12</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="I13" s="18" t="s">
+      <c r="I13" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J13" s="18" t="s">
+      <c r="J13" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K13" s="18" t="s">
+      <c r="K13" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="H14" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I14" s="20" t="s">
+      <c r="I14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J14" s="20" t="s">
+      <c r="J14" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="K14" s="20" t="s">
+      <c r="K14" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18">
+    <row r="15" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
         <v>14</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="I15" s="18" t="s">
+      <c r="I15" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J15" s="18" t="s">
+      <c r="J15" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="18" t="s">
+      <c r="K15" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18">
+    <row r="16" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
         <v>15</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="18" t="s">
+      <c r="H16" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="I16" s="18" t="s">
+      <c r="I16" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="18" t="s">
+      <c r="J16" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="K16" s="18" t="s">
+      <c r="K16" s="8" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Process variable changed from 16 bits to 32 bits. Added calculations of electrical current. Added moving average filter in the current value. Max and min sum of errors modified.
</commit_message>
<xml_diff>
--- a/Resources/DataPacket/Commands.xlsx
+++ b/Resources/DataPacket/Commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavi\Documents\Embed\STM32\Projects\CurrentController\Resources\DataPacket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6958DE-587E-458A-BFDD-A451A69D401B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C328C73-9800-4364-98DA-CE15F84E464E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Packet" sheetId="4" r:id="rId1"/>
@@ -303,9 +303,6 @@
     <t>Sets the value of delay PID: [0 : 65535] = [0x0000 : 0xFFFF]</t>
   </si>
   <si>
-    <t>Sets the value of Setpoint (electrical current in uA): [0 : 4294967295] = [0x00000000 : 0xFFFFFFFF]</t>
-  </si>
-  <si>
     <t>Sets the value of kp: [0 : 255] = [0x00 : 0xFF]</t>
   </si>
   <si>
@@ -315,7 +312,10 @@
     <t>Sets the value of kd: [0 : 255] = [0x00 : 0xFF]</t>
   </si>
   <si>
-    <t>Sends the current process variable value (electrical current in uA): [0 : 4294967295] = [0x00000000 : 0xFFFFFFFF]</t>
+    <t>Sets the value of Setpoint (electrical current in mA): [0 : 4294967295] = [0x00000000 : 0xFFFFFFFF]</t>
+  </si>
+  <si>
+    <t>Sends the current process variable value (electrical current in mA): [0 : 4294967295] = [0x00000000 : 0xFFFFFFFF]</t>
   </si>
 </sst>
 </file>
@@ -481,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -494,9 +494,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -840,14 +837,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -1412,13 +1409,13 @@
       <c r="AG6" s="3"/>
     </row>
     <row r="7" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -1449,11 +1446,11 @@
       <c r="AG7" s="3"/>
     </row>
     <row r="8" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="14"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1484,11 +1481,11 @@
       <c r="AG8" s="3"/>
     </row>
     <row r="9" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1519,11 +1516,11 @@
       <c r="AG9" s="3"/>
     </row>
     <row r="10" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="15"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -1554,11 +1551,11 @@
       <c r="AG10" s="3"/>
     </row>
     <row r="11" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="15"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="14"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -1589,11 +1586,11 @@
       <c r="AG11" s="3"/>
     </row>
     <row r="12" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="14"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -1624,11 +1621,11 @@
       <c r="AG12" s="3"/>
     </row>
     <row r="13" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="15"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="14"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -1659,11 +1656,11 @@
       <c r="AG13" s="3"/>
     </row>
     <row r="14" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="15"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="14"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1694,11 +1691,11 @@
       <c r="AG14" s="3"/>
     </row>
     <row r="15" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="15"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="14"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1729,11 +1726,11 @@
       <c r="AG15" s="3"/>
     </row>
     <row r="16" spans="1:369" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="18"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="17"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -40981,8 +40978,8 @@
   </sheetPr>
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41000,563 +40997,563 @@
     <col min="11" max="11" width="48.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="7" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+    <row r="2" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K3" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>2</v>
+    <row r="4" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>3</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>29</v>
+      <c r="B4" s="7" t="s">
+        <v>36</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>30</v>
+      <c r="E4" s="7" t="s">
+        <v>31</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>21</v>
+      <c r="H4" s="7" t="s">
+        <v>35</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J4" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K4" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>3</v>
+    <row r="5" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>4</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>36</v>
+      <c r="B5" s="7" t="s">
+        <v>38</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>31</v>
+      <c r="E5" s="7" t="s">
+        <v>32</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>35</v>
+      <c r="H7" s="7" t="s">
+        <v>47</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K13" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>4</v>
+    <row r="14" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>13</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>38</v>
+      <c r="B14" s="7" t="s">
+        <v>68</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>32</v>
+      <c r="E14" s="7" t="s">
+        <v>67</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F14" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="H15" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="K15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>37</v>
+    </row>
+    <row r="16" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>15</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="B16" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I16" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>5</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>6</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
-        <v>8</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
-        <v>9</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
-        <v>10</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
-        <v>11</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
-        <v>12</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
-        <v>14</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="K15" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>15</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J16" s="8" t="s">
+      <c r="J16" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="K16" s="7" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Current calculations and moving average filter moved from main to app file.
</commit_message>
<xml_diff>
--- a/Resources/DataPacket/Commands.xlsx
+++ b/Resources/DataPacket/Commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavi\Documents\Embed\STM32\Projects\CurrentController\Resources\DataPacket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C328C73-9800-4364-98DA-CE15F84E464E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6127D41D-4487-4E05-ACDD-A89C526D7C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -273,24 +273,6 @@
     <t>0x1B</t>
   </si>
   <si>
-    <t>Asks for the current sampling delay, PID delay, Setpoint values</t>
-  </si>
-  <si>
-    <t>Sends the current sampling delay, delay PID, Setpoint values</t>
-  </si>
-  <si>
-    <t>0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00</t>
-  </si>
-  <si>
-    <t>0xAA 0x55 0x17 0x08 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x8A</t>
-  </si>
-  <si>
-    <t>0x08</t>
-  </si>
-  <si>
-    <t>0x8A</t>
-  </si>
-  <si>
     <t>Disables the send of the current process variable value (electrical current in uA) from microcontroller to PC at each 100ms</t>
   </si>
   <si>
@@ -316,6 +298,24 @@
   </si>
   <si>
     <t>Sends the current process variable value (electrical current in mA): [0 : 4294967295] = [0x00000000 : 0xFFFFFFFF]</t>
+  </si>
+  <si>
+    <t>Asks for the current sampling delay, PID delay, Setpoint, Moving Average Window values</t>
+  </si>
+  <si>
+    <t>Sends the current sampling delay, delay PID, Setpoint, Moving Average Window values</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x17 0x09 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0xD7</t>
+  </si>
+  <si>
+    <t>0x09</t>
+  </si>
+  <si>
+    <t>0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00</t>
+  </si>
+  <si>
+    <t>0xD7</t>
   </si>
 </sst>
 </file>
@@ -481,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -535,6 +535,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -40978,19 +40982,19 @@
   </sheetPr>
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="97.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -41061,7 +41065,7 @@
         <v>26</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>24</v>
@@ -41096,7 +41100,7 @@
         <v>26</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>24</v>
@@ -41131,7 +41135,7 @@
         <v>26</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>24</v>
@@ -41306,44 +41310,44 @@
         <v>26</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+    <row r="10" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="19">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>78</v>
+      <c r="B10" s="19" t="s">
+        <v>86</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>79</v>
+      <c r="F10" s="19" t="s">
+        <v>87</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>77</v>
+      <c r="G10" s="19" t="s">
+        <v>88</v>
       </c>
-      <c r="H10" s="7" t="s">
-        <v>80</v>
+      <c r="H10" s="19" t="s">
+        <v>89</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="7" t="s">
-        <v>76</v>
+      <c r="J10" s="19" t="s">
+        <v>85</v>
       </c>
-      <c r="K10" s="7" t="s">
+      <c r="K10" s="19" t="s">
         <v>24</v>
       </c>
     </row>
@@ -41376,7 +41380,7 @@
         <v>26</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>24</v>
@@ -41411,7 +41415,7 @@
         <v>26</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>24</v>
@@ -41446,7 +41450,7 @@
         <v>26</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>24</v>
@@ -41481,7 +41485,7 @@
         <v>27</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>24</v>
@@ -41516,7 +41520,7 @@
         <v>26</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>18</v>
@@ -41551,7 +41555,7 @@
         <v>26</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Send the value of moving average filter window to computer.
</commit_message>
<xml_diff>
--- a/Resources/DataPacket/Commands.xlsx
+++ b/Resources/DataPacket/Commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavi\Documents\Embed\STM32\Projects\CurrentController\Resources\DataPacket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6127D41D-4487-4E05-ACDD-A89C526D7C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BF7CE1-4B1D-444F-B913-E9470D0B1B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -481,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -535,10 +535,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -40982,8 +40978,8 @@
   </sheetPr>
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41316,38 +41312,38 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="19">
+    <row r="10" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="I10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="K10" s="19" t="s">
+      <c r="K10" s="7" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added functionality of receive and set the moving average window.
</commit_message>
<xml_diff>
--- a/Resources/DataPacket/Commands.xlsx
+++ b/Resources/DataPacket/Commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavi\Documents\Embed\STM32\Projects\CurrentController\Resources\DataPacket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BF7CE1-4B1D-444F-B913-E9470D0B1B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AE1804-1000-4C0E-8A53-4175FA7B59F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Commands" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Commands!$A$1:$K$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Commands!$A$1:$K$17</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Commands!$A$1:$K$18</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Data Packet'!$A$1:$F$18</definedName>
   </definedNames>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="92">
   <si>
     <t>Start byte 1</t>
   </si>
@@ -111,13 +111,7 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>0x40</t>
-  </si>
-  <si>
     <t>0x01</t>
-  </si>
-  <si>
-    <t>0x2B</t>
   </si>
   <si>
     <t>The CRC8 is dependent of the payload. Payload is not fixed.</t>
@@ -130,12 +124,6 @@
   </si>
   <si>
     <t>From Microcontroller to PC</t>
-  </si>
-  <si>
-    <t>0xAA 0x55 0x10 0x01 0x00 0x2B</t>
-  </si>
-  <si>
-    <t>0xAA 0x55 0x11 0x01 0x00 0x40</t>
   </si>
   <si>
     <t>0x11</t>
@@ -153,12 +141,6 @@
     <t>Sends the current kp, ki and kd values</t>
   </si>
   <si>
-    <t>0xFD</t>
-  </si>
-  <si>
-    <t>0xAA 0x55 0x12 0x01 0x00 0xFD</t>
-  </si>
-  <si>
     <t>0xEF</t>
   </si>
   <si>
@@ -166,18 +148,6 @@
   </si>
   <si>
     <t>0x14</t>
-  </si>
-  <si>
-    <t>0x00 0x00 0x00</t>
-  </si>
-  <si>
-    <t>0x03</t>
-  </si>
-  <si>
-    <t>0x9A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0xAA 0x55 0x14 0x03 0x00 0x00 0x00 0x9A </t>
   </si>
   <si>
     <t>0x15</t>
@@ -279,50 +249,86 @@
     <t>Enables the send of the current process variable value (electrical current in uA) from microcontroller to PC at each 100ms</t>
   </si>
   <si>
-    <t>Sets the value of sampling delay: [0 : 65535] = [0x0000 : 0xFFFF]</t>
-  </si>
-  <si>
-    <t>Sets the value of delay PID: [0 : 65535] = [0x0000 : 0xFFFF]</t>
-  </si>
-  <si>
-    <t>Sets the value of kp: [0 : 255] = [0x00 : 0xFF]</t>
-  </si>
-  <si>
-    <t>Sets the value of ki: [0 : 255] = [0x00 : 0xFF]</t>
-  </si>
-  <si>
-    <t>Sets the value of kd: [0 : 255] = [0x00 : 0xFF]</t>
-  </si>
-  <si>
     <t>Sets the value of Setpoint (electrical current in mA): [0 : 4294967295] = [0x00000000 : 0xFFFFFFFF]</t>
   </si>
   <si>
     <t>Sends the current process variable value (electrical current in mA): [0 : 4294967295] = [0x00000000 : 0xFFFFFFFF]</t>
   </si>
   <si>
-    <t>Asks for the current sampling delay, PID delay, Setpoint, Moving Average Window values</t>
+    <t>Asks for the current sampling interval, PID interval, Setpoint, Moving Average Window values</t>
   </si>
   <si>
-    <t>Sends the current sampling delay, delay PID, Setpoint, Moving Average Window values</t>
+    <t>Sends the current sampling interval, interval PID, Setpoint, Moving Average Window values</t>
   </si>
   <si>
-    <t>0xAA 0x55 0x17 0x09 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0xD7</t>
+    <t>Sets the value of sampling interval: [0 : 65535] = [0x0000 : 0xFFFF]</t>
   </si>
   <si>
-    <t>0x09</t>
+    <t>Sets the value of interval PID: [0 : 65535] = [0x0000 : 0xFFFF]</t>
   </si>
   <si>
-    <t>0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00</t>
+    <t>Sets the value of kp: [0 : 4294967295] = [0x00000000 : 0xFFFFFFFF]</t>
   </si>
   <si>
-    <t>0xD7</t>
+    <t>Sets the value of ki: [0 : 4294967295] = [0x00000000 : 0xFFFFFFFF]</t>
+  </si>
+  <si>
+    <t>Sets the value of kd: [0 : 4294967295] = [0x00000000 : 0xFFFFFFFF]</t>
+  </si>
+  <si>
+    <t>0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xAA 0x55 0x10 0x04 0x00 0x00 0x00 0x00 0x42 </t>
+  </si>
+  <si>
+    <t>0x42</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x11 0x04 0x00 0x00 0x00 0x00 0x6B</t>
+  </si>
+  <si>
+    <t>0x6B</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x12 0x04 0x00 0x00 0x00 0x00 0x10</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x14 0x0C 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0xDB</t>
+  </si>
+  <si>
+    <t>0x0C</t>
+  </si>
+  <si>
+    <t>0xDB</t>
+  </si>
+  <si>
+    <t>Sets the value of moving average window: [0 : 255] = [0x00 : 0xFF]</t>
+  </si>
+  <si>
+    <t>0x23</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x23 0x02 0x00 0x00 0xFF</t>
+  </si>
+  <si>
+    <t>0xFF</t>
+  </si>
+  <si>
+    <t>0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x17 0x0A 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x0A</t>
+  </si>
+  <si>
+    <t>0x0A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,6 +361,12 @@
       <b/>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -481,7 +493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -535,6 +547,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -40976,21 +40992,21 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="66.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="34.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="97.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -41023,7 +41039,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>12</v>
@@ -41037,7 +41053,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>14</v>
@@ -41049,22 +41065,22 @@
         <v>16</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -41072,7 +41088,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>14</v>
@@ -41081,25 +41097,25 @@
         <v>15</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -41107,7 +41123,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>14</v>
@@ -41116,25 +41132,25 @@
         <v>15</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -41142,7 +41158,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>14</v>
@@ -41151,7 +41167,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>17</v>
@@ -41160,13 +41176,13 @@
         <v>18</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>18</v>
@@ -41177,7 +41193,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>14</v>
@@ -41186,25 +41202,25 @@
         <v>15</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -41212,7 +41228,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>14</v>
@@ -41221,22 +41237,22 @@
         <v>15</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>17</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>18</v>
@@ -41247,7 +41263,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>14</v>
@@ -41256,22 +41272,22 @@
         <v>15</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>18</v>
@@ -41282,7 +41298,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>14</v>
@@ -41291,7 +41307,7 @@
         <v>15</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>17</v>
@@ -41300,13 +41316,13 @@
         <v>18</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>18</v>
@@ -41317,7 +41333,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>14</v>
@@ -41326,25 +41342,25 @@
         <v>15</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -41352,7 +41368,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>14</v>
@@ -41361,25 +41377,25 @@
         <v>15</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -41387,7 +41403,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>14</v>
@@ -41396,25 +41412,25 @@
         <v>15</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -41422,7 +41438,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>14</v>
@@ -41434,22 +41450,22 @@
         <v>19</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -41457,7 +41473,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>14</v>
@@ -41466,25 +41482,25 @@
         <v>15</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -41492,7 +41508,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>14</v>
@@ -41501,22 +41517,22 @@
         <v>15</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>17</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>18</v>
@@ -41527,7 +41543,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>14</v>
@@ -41536,29 +41552,64 @@
         <v>15</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>18</v>
       </c>
     </row>
+    <row r="17" spans="1:11" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A17" s="19">
+        <v>16</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="K17" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K16" xr:uid="{B11DB8B0-5B17-4A82-8032-D4706BCA4450}"/>
+  <autoFilter ref="A1:K17" xr:uid="{B11DB8B0-5B17-4A82-8032-D4706BCA4450}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup scale="39" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added functionality of send min and max sum of errors and controlled variable.
</commit_message>
<xml_diff>
--- a/Resources/DataPacket/Commands.xlsx
+++ b/Resources/DataPacket/Commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavi\Documents\Embed\STM32\Projects\CurrentController\Resources\DataPacket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AE1804-1000-4C0E-8A53-4175FA7B59F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203B1AB5-4308-4551-A734-4A6111D2B485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="109">
   <si>
     <t>Start byte 1</t>
   </si>
@@ -323,6 +323,57 @@
   <si>
     <t>0x0A</t>
   </si>
+  <si>
+    <t>Asks for min and max sum of errors</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x24 0x00 0x7D</t>
+  </si>
+  <si>
+    <t>0x24</t>
+  </si>
+  <si>
+    <t>0x7D</t>
+  </si>
+  <si>
+    <t>Sends the current min and max sum of errors values</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x25 0x08 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0xEB</t>
+  </si>
+  <si>
+    <t>0x25</t>
+  </si>
+  <si>
+    <t>0x08</t>
+  </si>
+  <si>
+    <t>0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00</t>
+  </si>
+  <si>
+    <t>Asks for min and max controlled variable</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x26 0x00 0x57</t>
+  </si>
+  <si>
+    <t>0x26</t>
+  </si>
+  <si>
+    <t>0x57</t>
+  </si>
+  <si>
+    <t>Sends the current min and max controlled variable</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x27 0x08 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x3B</t>
+  </si>
+  <si>
+    <t>0x27</t>
+  </si>
+  <si>
+    <t>0x3B</t>
+  </si>
 </sst>
 </file>
 
@@ -493,7 +544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -517,6 +568,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -547,10 +602,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -853,14 +907,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -1425,13 +1479,13 @@
       <c r="AG6" s="3"/>
     </row>
     <row r="7" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -1462,11 +1516,11 @@
       <c r="AG7" s="3"/>
     </row>
     <row r="8" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="16"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1497,11 +1551,11 @@
       <c r="AG8" s="3"/>
     </row>
     <row r="9" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="16"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1532,11 +1586,11 @@
       <c r="AG9" s="3"/>
     </row>
     <row r="10" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="16"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -1567,11 +1621,11 @@
       <c r="AG10" s="3"/>
     </row>
     <row r="11" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="16"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -1602,11 +1656,11 @@
       <c r="AG11" s="3"/>
     </row>
     <row r="12" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="16"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -1637,11 +1691,11 @@
       <c r="AG12" s="3"/>
     </row>
     <row r="13" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -1672,11 +1726,11 @@
       <c r="AG13" s="3"/>
     </row>
     <row r="14" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="14"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="16"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1707,11 +1761,11 @@
       <c r="AG14" s="3"/>
     </row>
     <row r="15" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="16"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1742,11 +1796,11 @@
       <c r="AG15" s="3"/>
     </row>
     <row r="16" spans="1:369" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="17"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="19"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -40992,10 +41046,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41573,40 +41627,323 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A17" s="19">
+    <row r="17" spans="1:11" s="10" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
         <v>16</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="F17" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="19" t="s">
+      <c r="H17" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="I17" s="19" t="s">
+      <c r="I17" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="19" t="s">
+      <c r="J17" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="K17" s="19" t="s">
+      <c r="K17" s="9" t="s">
         <v>22</v>
       </c>
+    </row>
+    <row r="18" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>17</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>18</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>19</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>20</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="21"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="21"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:K17" xr:uid="{B11DB8B0-5B17-4A82-8032-D4706BCA4450}"/>

</xml_diff>

<commit_message>
Added functionality of receive the min and max sum of errors and controlled variable.
</commit_message>
<xml_diff>
--- a/Resources/DataPacket/Commands.xlsx
+++ b/Resources/DataPacket/Commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavi\Documents\Embed\STM32\Projects\CurrentController\Resources\DataPacket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203B1AB5-4308-4551-A734-4A6111D2B485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73521F4-E580-434D-BEEA-58AEBC3261DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="125">
   <si>
     <t>Start byte 1</t>
   </si>
@@ -303,9 +303,6 @@
     <t>0xDB</t>
   </si>
   <si>
-    <t>Sets the value of moving average window: [0 : 255] = [0x00 : 0xFF]</t>
-  </si>
-  <si>
     <t>0x23</t>
   </si>
   <si>
@@ -373,6 +370,57 @@
   </si>
   <si>
     <t>0x3B</t>
+  </si>
+  <si>
+    <t>Sets the value of moving average window: [0 : 65535] = [0x0000 : 0xFFFF]</t>
+  </si>
+  <si>
+    <t>Sets the value of min sum of errors: [0 : 4294967295] = [0x00000000 : 0xFFFFFFFF]</t>
+  </si>
+  <si>
+    <t>Sets the value of max sum of errors: [0 : 4294967295] = [0x00000000 : 0xFFFFFFFF]</t>
+  </si>
+  <si>
+    <t>Sets the value of min controlled variable: [0 : 4294967295] = [0x00000000 : 0xFFFFFFFF]</t>
+  </si>
+  <si>
+    <t>Sets the value of max controlled variable: [0 : 4294967295] = [0x00000000 : 0xFFFFFFFF]</t>
+  </si>
+  <si>
+    <t>0x28</t>
+  </si>
+  <si>
+    <t>0x29</t>
+  </si>
+  <si>
+    <t>0x30</t>
+  </si>
+  <si>
+    <t>0x31</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x28 0x04 0x00 0x00 0x00 0x00 0xA8</t>
+  </si>
+  <si>
+    <t>0xA8</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x29 0x04 0x00 0x00 0x00 0x00 0x81</t>
+  </si>
+  <si>
+    <t>0x81</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x30 0x04 0x00 0x00 0x00 0x00 0x79</t>
+  </si>
+  <si>
+    <t>0x79</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x31 0x04 0x00 0x00 0x00 0x00 0x50</t>
+  </si>
+  <si>
+    <t>0x50</t>
   </si>
 </sst>
 </file>
@@ -572,6 +620,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -601,9 +652,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -907,14 +955,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -1479,13 +1527,13 @@
       <c r="AG6" s="3"/>
     </row>
     <row r="7" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -1516,11 +1564,11 @@
       <c r="AG7" s="3"/>
     </row>
     <row r="8" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="16"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1551,11 +1599,11 @@
       <c r="AG8" s="3"/>
     </row>
     <row r="9" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="16"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1586,11 +1634,11 @@
       <c r="AG9" s="3"/>
     </row>
     <row r="10" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="16"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="17"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -1621,11 +1669,11 @@
       <c r="AG10" s="3"/>
     </row>
     <row r="11" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="16"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -1656,11 +1704,11 @@
       <c r="AG11" s="3"/>
     </row>
     <row r="12" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -1691,11 +1739,11 @@
       <c r="AG12" s="3"/>
     </row>
     <row r="13" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="16"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="17"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -1726,11 +1774,11 @@
       <c r="AG13" s="3"/>
     </row>
     <row r="14" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="16"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="17"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1761,11 +1809,11 @@
       <c r="AG14" s="3"/>
     </row>
     <row r="15" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="17"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1796,11 +1844,11 @@
       <c r="AG15" s="3"/>
     </row>
     <row r="16" spans="1:369" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="19"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -41048,8 +41096,8 @@
   </sheetPr>
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41387,7 +41435,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>14</v>
@@ -41399,13 +41447,13 @@
         <v>44</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>25</v>
@@ -41632,7 +41680,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>14</v>
@@ -41641,7 +41689,7 @@
         <v>15</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>48</v>
@@ -41650,13 +41698,13 @@
         <v>46</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I17" s="9" t="s">
         <v>24</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>22</v>
@@ -41667,7 +41715,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>14</v>
@@ -41676,7 +41724,7 @@
         <v>15</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>17</v>
@@ -41685,13 +41733,13 @@
         <v>18</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I18" s="7" t="s">
         <v>24</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>18</v>
@@ -41702,7 +41750,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>14</v>
@@ -41711,13 +41759,13 @@
         <v>15</v>
       </c>
       <c r="E19" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="G19" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>100</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>37</v>
@@ -41726,7 +41774,7 @@
         <v>25</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>22</v>
@@ -41737,7 +41785,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>14</v>
@@ -41746,7 +41794,7 @@
         <v>15</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>17</v>
@@ -41755,13 +41803,13 @@
         <v>18</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I20" s="7" t="s">
         <v>24</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>18</v>
@@ -41772,7 +41820,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>14</v>
@@ -41781,169 +41829,257 @@
         <v>15</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F21" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="G21" s="7" t="s">
-        <v>100</v>
-      </c>
       <c r="H21" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I21" s="7" t="s">
         <v>25</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="21"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
+    <row r="22" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>21</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>22</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>23</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>24</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="21"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="21"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="21"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="21"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
-      <c r="K32" s="21"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:K17" xr:uid="{B11DB8B0-5B17-4A82-8032-D4706BCA4450}"/>

</xml_diff>

<commit_message>
Added functionality of send current pid offset and bias.
</commit_message>
<xml_diff>
--- a/Resources/DataPacket/Commands.xlsx
+++ b/Resources/DataPacket/Commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavi\Documents\Embed\STM32\Projects\CurrentController\Resources\DataPacket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73521F4-E580-434D-BEEA-58AEBC3261DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95183C36-C91F-4EDF-A60A-F5FD8DA24E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="141">
   <si>
     <t>Start byte 1</t>
   </si>
@@ -422,6 +422,54 @@
   <si>
     <t>0x50</t>
   </si>
+  <si>
+    <t>Asks for PID offset and PID Bias</t>
+  </si>
+  <si>
+    <t>Sends the PID offset and PID Bias</t>
+  </si>
+  <si>
+    <t>Sets the value of PID Offset: [0 : 4294967295] = [0x00000000 : 0xFFFFFFFF]</t>
+  </si>
+  <si>
+    <t>Sets the value of PID Bias: [0 : 4294967295] = [0x00000000 : 0xFFFFFFFF]</t>
+  </si>
+  <si>
+    <t>0x32</t>
+  </si>
+  <si>
+    <t>0x33</t>
+  </si>
+  <si>
+    <t>0x34</t>
+  </si>
+  <si>
+    <t>0x35</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x32 0x00 0x54</t>
+  </si>
+  <si>
+    <t>0x54</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x33 0x08 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x0E</t>
+  </si>
+  <si>
+    <t>0x0E</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x34 0x04 0x00 0x00 0x00 0x00 0xDD</t>
+  </si>
+  <si>
+    <t>0xDD</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x35 0x04 0x00 0x00 0x00 0x00 0xF4</t>
+  </si>
+  <si>
+    <t>0xF4</t>
+  </si>
 </sst>
 </file>
 
@@ -592,7 +640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -652,6 +700,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -41096,8 +41147,8 @@
   </sheetPr>
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41109,8 +41160,8 @@
     <col min="5" max="5" width="8.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" style="1" customWidth="1"/>
     <col min="10" max="10" width="97.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="48.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
@@ -41990,57 +42041,145 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
+    <row r="26" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>25</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>26</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
+      <c r="A28" s="22">
+        <v>27</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="H28" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="I28" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="J28" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="K28" s="22" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
+      <c r="A29" s="22">
+        <v>28</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="F29" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="G29" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="H29" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="I29" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="J29" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="K29" s="22" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>

</xml_diff>

<commit_message>
DAC output buffer disabled.
</commit_message>
<xml_diff>
--- a/Resources/DataPacket/Commands.xlsx
+++ b/Resources/DataPacket/Commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavi\Documents\Embed\STM32\Projects\CurrentController\Resources\DataPacket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95183C36-C91F-4EDF-A60A-F5FD8DA24E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1749B318-B23D-4805-A74B-192B8BDC6BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -640,7 +640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -700,9 +700,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -41147,8 +41144,8 @@
   </sheetPr>
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42111,73 +42108,73 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="22">
+    <row r="28" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
         <v>27</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="22" t="s">
+      <c r="D28" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="22" t="s">
+      <c r="E28" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="F28" s="22" t="s">
+      <c r="F28" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G28" s="22" t="s">
+      <c r="G28" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="H28" s="22" t="s">
+      <c r="H28" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="I28" s="22" t="s">
+      <c r="I28" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="J28" s="22" t="s">
+      <c r="J28" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="K28" s="22" t="s">
+      <c r="K28" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="22">
+    <row r="29" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
         <v>28</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="22" t="s">
+      <c r="D29" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="22" t="s">
+      <c r="E29" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="F29" s="22" t="s">
+      <c r="F29" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G29" s="22" t="s">
+      <c r="G29" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="H29" s="22" t="s">
+      <c r="H29" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="I29" s="22" t="s">
+      <c r="I29" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="J29" s="22" t="s">
+      <c r="J29" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="K29" s="22" t="s">
+      <c r="K29" s="7" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed the shape of packets of serial communication.
</commit_message>
<xml_diff>
--- a/Resources/DataPacket/Commands.xlsx
+++ b/Resources/DataPacket/Commands.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavi\Documents\Embed\STM32\Projects\CurrentController\Resources\DataPacket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1749B318-B23D-4805-A74B-192B8BDC6BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A38085-32FD-49F6-89B0-A4930732163A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Packet" sheetId="4" r:id="rId1"/>
-    <sheet name="Commands" sheetId="5" r:id="rId2"/>
+    <sheet name="Commands v0.1" sheetId="5" r:id="rId2"/>
+    <sheet name="Commands v0.2" sheetId="6" r:id="rId3"/>
+    <sheet name="Config data" sheetId="7" r:id="rId4"/>
+    <sheet name="Config data (2)" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Commands!$A$1:$K$17</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Commands!$A$1:$K$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Commands v0.1'!$A$1:$K$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Commands v0.2'!$A$1:$K$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Commands v0.1'!$A$1:$K$18</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Commands v0.2'!$A$1:$K$14</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Data Packet'!$A$1:$F$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -42,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="250">
   <si>
     <t>Start byte 1</t>
   </si>
@@ -470,12 +475,350 @@
   <si>
     <t>0xF4</t>
   </si>
+  <si>
+    <t>Sets the value of configuration data:
+[kp (4 bytes) | ki (4 bytes) | kd (4 bytes) | PID Interval (2 bytes) | Sampling Interval (2 bytes) | Moving Average Window (2 bytes) | Min Sum of Errors (4 bytes) | Max Sum of Errors (4 bytes) | Min Controlled Variable (4 bytes) | Max Controlled Variable (4 bytes) | PID Offset (4 bytes) | PID Bias (4 bytes)]</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x01 0x2A 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x8D</t>
+  </si>
+  <si>
+    <t>0x2A</t>
+  </si>
+  <si>
+    <t>0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00</t>
+  </si>
+  <si>
+    <t>0x8D</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x02 0x00 0xAD</t>
+  </si>
+  <si>
+    <t>0xAD</t>
+  </si>
+  <si>
+    <t>0x03</t>
+  </si>
+  <si>
+    <t>Sets the value of PID Setpoint (electrical current in mA):
+(4 bytes) = [0 : 4294967295] = [0x00000000 : 0xFFFFFFFF]</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x03 0x04 0x00 0x00 0x00 0x00 0xA7</t>
+  </si>
+  <si>
+    <t>0xA7</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x04 0x01 0x01 0x25</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x04 0x01 0x00 0x22</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x05 0x01 0x00 0x49</t>
+  </si>
+  <si>
+    <t>0x05</t>
+  </si>
+  <si>
+    <t>0x49</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x05 0x01 0x01 0x4E</t>
+  </si>
+  <si>
+    <t>0x4E</t>
+  </si>
+  <si>
+    <t>RESERVED</t>
+  </si>
+  <si>
+    <t>FREE</t>
+  </si>
+  <si>
+    <t>0x06 - 0x7F</t>
+  </si>
+  <si>
+    <t>0x80</t>
+  </si>
+  <si>
+    <t>Asks for the current value of configuration data:
+[kp | ki  | kd | PID Interval | Sampling Interval | Moving Average Window | Min Sum of Errors | Max Sum of Errors | Min Controlled Variable | Max Controlled Variable | PID Offset | PID Bias]</t>
+  </si>
+  <si>
+    <t>Sends the current value of configuration data:
+[kp (4 bytes) | ki (4 bytes) | kd (4 bytes) | PID Interval (2 bytes) | Sampling Interval (2 bytes) | Moving Average Window (2 bytes) | Min Sum of Errors (4 bytes) | Max Sum of Errors (4 bytes) | Min Controlled Variable (4 bytes) | Max Controlled Variable (4 bytes) | PID Offset (4 bytes) | PID Bias (4 bytes)]</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x80 0x2A 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0xD1</t>
+  </si>
+  <si>
+    <t>0xD1</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x81 0x04 0x00 0x00 0x00 0x00 0x19</t>
+  </si>
+  <si>
+    <t>0x82</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x82 0x04 0x00 0x00 0x00 0x00 0x62</t>
+  </si>
+  <si>
+    <t>0x62</t>
+  </si>
+  <si>
+    <t>Sends the current process variable value (electrical current in mA):
+(4 byter) = [0 : 4294967295] = [0x00000000 : 0xFFFFFFFF]</t>
+  </si>
+  <si>
+    <t>0x83 - 0xFE</t>
+  </si>
+  <si>
+    <t>0XFF</t>
+  </si>
+  <si>
+    <t>Sends the current value of PID Setpoint (electrical current in mA):
+(4 bytes) = [0 : 4294967295] = [0x00000000 : 0xFFFFFFFF]</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Kp</t>
+  </si>
+  <si>
+    <t>Ki</t>
+  </si>
+  <si>
+    <t>Kd</t>
+  </si>
+  <si>
+    <t>PID Interval</t>
+  </si>
+  <si>
+    <t>Sampling Interval</t>
+  </si>
+  <si>
+    <t>Qty bytes</t>
+  </si>
+  <si>
+    <t>Moving Average Window</t>
+  </si>
+  <si>
+    <t>Min Sum of Errors</t>
+  </si>
+  <si>
+    <t>Max Sum of Errors</t>
+  </si>
+  <si>
+    <t>Min Controlled Variable</t>
+  </si>
+  <si>
+    <t>Max Controlled Variable</t>
+  </si>
+  <si>
+    <t>PID Offset</t>
+  </si>
+  <si>
+    <t>PID Bias</t>
+  </si>
+  <si>
+    <t>Total bytes</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>f1</t>
+  </si>
+  <si>
+    <t>Byte 1 [HEX]</t>
+  </si>
+  <si>
+    <t>Byte 2 [HEX]</t>
+  </si>
+  <si>
+    <t>Byte 3 [HEX]</t>
+  </si>
+  <si>
+    <t>Byte 4 [HEX]</t>
+  </si>
+  <si>
+    <t>Data [HEX]</t>
+  </si>
+  <si>
+    <t>Data [DEC]</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>bc</t>
+  </si>
+  <si>
+    <t>e0</t>
+  </si>
+  <si>
+    <t>ff</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>ea</t>
+  </si>
+  <si>
+    <t>ae</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>ee</t>
+  </si>
+  <si>
+    <t>ab</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>Calc [DEC]</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>Byte 0 [HEX]
+(just to complete the 40 bytes required by excel)</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>ed</t>
+  </si>
+  <si>
+    <t>ad</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>6a</t>
+  </si>
+  <si>
+    <t>2b</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>D0</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>FA</t>
+  </si>
+  <si>
+    <t>3B</t>
+  </si>
+  <si>
+    <t>9A</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>F0</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>0F</t>
+  </si>
+  <si>
+    <t>4A</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="#,##0.000"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -518,8 +861,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -532,8 +882,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -636,11 +998,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -671,6 +1113,49 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -699,6 +1184,42 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1003,14 +1524,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -1575,13 +2096,13 @@
       <c r="AG6" s="3"/>
     </row>
     <row r="7" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="29"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -1612,11 +2133,11 @@
       <c r="AG7" s="3"/>
     </row>
     <row r="8" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="17"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="32"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1647,11 +2168,11 @@
       <c r="AG8" s="3"/>
     </row>
     <row r="9" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="17"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="32"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1682,11 +2203,11 @@
       <c r="AG9" s="3"/>
     </row>
     <row r="10" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="32"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -1717,11 +2238,11 @@
       <c r="AG10" s="3"/>
     </row>
     <row r="11" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="17"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="32"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -1752,11 +2273,11 @@
       <c r="AG11" s="3"/>
     </row>
     <row r="12" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="17"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -1787,11 +2308,11 @@
       <c r="AG12" s="3"/>
     </row>
     <row r="13" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="17"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="32"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -1822,11 +2343,11 @@
       <c r="AG13" s="3"/>
     </row>
     <row r="14" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="17"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="32"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1857,11 +2378,11 @@
       <c r="AG14" s="3"/>
     </row>
     <row r="15" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="17"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="32"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1892,11 +2413,11 @@
       <c r="AG15" s="3"/>
     </row>
     <row r="16" spans="1:369" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="20"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="35"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -41144,8 +41665,8 @@
   </sheetPr>
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42218,8 +42739,1647 @@
       <c r="K32" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K17" xr:uid="{B11DB8B0-5B17-4A82-8032-D4706BCA4450}"/>
+  <autoFilter ref="A1:K29" xr:uid="{B11DB8B0-5B17-4A82-8032-D4706BCA4450}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup scale="39" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5AB657F-0BAD-4DF8-BA58-E07351F31F9C}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:K18"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="58.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="121.42578125" style="15" customWidth="1"/>
+    <col min="11" max="11" width="48.28515625" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="18" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="18" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="18" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
+        <v>4</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="18" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
+        <v>10</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="K11" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="18" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
+        <v>11</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="18" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A13" s="16">
+        <v>12</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="K13" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A14" s="12">
+        <v>13</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A15" s="12">
+        <v>14</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="11"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="11"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="11"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:K15" xr:uid="{B11DB8B0-5B17-4A82-8032-D4706BCA4450}"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup scale="39" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E317EF53-64C8-4E32-A53D-867BE06A0082}">
+  <dimension ref="A1:R14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="28.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" style="41" customWidth="1"/>
+    <col min="5" max="8" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="17" style="37" customWidth="1"/>
+    <col min="12" max="18" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="H1" s="43" t="s">
+        <v>195</v>
+      </c>
+      <c r="I1" s="38" t="s">
+        <v>196</v>
+      </c>
+      <c r="J1" s="38" t="s">
+        <v>197</v>
+      </c>
+      <c r="K1" s="45" t="s">
+        <v>219</v>
+      </c>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2" s="24">
+        <v>4</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="H2" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="I2" s="39" t="str">
+        <f>_xlfn.CONCAT(D2:H2)</f>
+        <v>00000085f1</v>
+      </c>
+      <c r="J2" s="39">
+        <f>HEX2DEC(I2)</f>
+        <v>34289</v>
+      </c>
+      <c r="K2" s="46">
+        <f>J2/1000</f>
+        <v>34.289000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="24">
+        <v>4</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>211</v>
+      </c>
+      <c r="H3" s="44" t="s">
+        <v>224</v>
+      </c>
+      <c r="I3" s="39" t="str">
+        <f t="shared" ref="I3:I13" si="0">_xlfn.CONCAT(D3:H3)</f>
+        <v>000000ea48</v>
+      </c>
+      <c r="J3" s="39">
+        <f t="shared" ref="J3:J13" si="1">HEX2DEC(I3)</f>
+        <v>59976</v>
+      </c>
+      <c r="K3" s="46">
+        <f>J3/1000</f>
+        <v>59.975999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" s="24">
+        <v>4</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="H4" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="I4" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>00000079ed</v>
+      </c>
+      <c r="J4" s="39">
+        <f t="shared" si="1"/>
+        <v>31213</v>
+      </c>
+      <c r="K4" s="46">
+        <f>J4/1000</f>
+        <v>31.213000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C5" s="24">
+        <v>2</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="G5" s="26"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>001546</v>
+      </c>
+      <c r="J5" s="39">
+        <f t="shared" si="1"/>
+        <v>5446</v>
+      </c>
+      <c r="K5" s="47">
+        <f>INT(J5/10)</f>
+        <v>544</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" s="24">
+        <v>2</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="G6" s="26"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>00adbc</v>
+      </c>
+      <c r="J6" s="39">
+        <f t="shared" si="1"/>
+        <v>44476</v>
+      </c>
+      <c r="K6" s="47">
+        <f>INT(J6/10)</f>
+        <v>4447</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C7" s="24">
+        <v>2</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="G7" s="26"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>002143</v>
+      </c>
+      <c r="J7" s="39">
+        <f t="shared" si="1"/>
+        <v>8515</v>
+      </c>
+      <c r="K7" s="47">
+        <f>INT(J7)</f>
+        <v>8515</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C8" s="24">
+        <v>4</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="H8" s="44" t="s">
+        <v>206</v>
+      </c>
+      <c r="I8" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>0000e0ff54</v>
+      </c>
+      <c r="J8" s="39">
+        <f t="shared" si="1"/>
+        <v>14745428</v>
+      </c>
+      <c r="K8" s="47">
+        <f>INT(J8-1000000000)</f>
+        <v>-985254572</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C9" s="24">
+        <v>4</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>230</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="H9" s="44" t="s">
+        <v>207</v>
+      </c>
+      <c r="I9" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>006a052010</v>
+      </c>
+      <c r="J9" s="39">
+        <f t="shared" si="1"/>
+        <v>1778720784</v>
+      </c>
+      <c r="K9" s="47">
+        <f>INT(J9-1000000000)</f>
+        <v>778720784</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C10" s="24">
+        <v>4</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="H10" s="44" t="s">
+        <v>210</v>
+      </c>
+      <c r="I10" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>0064980200</v>
+      </c>
+      <c r="J10" s="39">
+        <f t="shared" si="1"/>
+        <v>1687683584</v>
+      </c>
+      <c r="K10" s="47">
+        <f>INT(J10-1000000000)</f>
+        <v>687683584</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C11" s="24">
+        <v>4</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="H11" s="44" t="s">
+        <v>214</v>
+      </c>
+      <c r="I11" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>002bae4080</v>
+      </c>
+      <c r="J11" s="39">
+        <f t="shared" si="1"/>
+        <v>732840064</v>
+      </c>
+      <c r="K11" s="47">
+        <f>INT(J11-1000000000)</f>
+        <v>-267159936</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C12" s="24">
+        <v>4</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="H12" s="44" t="s">
+        <v>217</v>
+      </c>
+      <c r="I12" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>002812eeab</v>
+      </c>
+      <c r="J12" s="39">
+        <f t="shared" si="1"/>
+        <v>672329387</v>
+      </c>
+      <c r="K12" s="48">
+        <f>(J12-1000000)/1000</f>
+        <v>671329.38699999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C13" s="24">
+        <v>4</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="G13" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="H13" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="I13" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>0000000056</v>
+      </c>
+      <c r="J13" s="39">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="K13" s="46">
+        <f>(J13-1000000)/1000</f>
+        <v>-999.91399999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="C14" s="3">
+        <f>SUM(C2:C13)</f>
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F1C60FF-9CA3-4972-9764-D5189C56A132}">
+  <dimension ref="A1:R14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="28.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" style="41" customWidth="1"/>
+    <col min="5" max="8" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="17" style="37" customWidth="1"/>
+    <col min="12" max="18" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="H1" s="43" t="s">
+        <v>195</v>
+      </c>
+      <c r="I1" s="38" t="s">
+        <v>196</v>
+      </c>
+      <c r="J1" s="38" t="s">
+        <v>197</v>
+      </c>
+      <c r="K1" s="45" t="s">
+        <v>219</v>
+      </c>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2" s="24">
+        <v>4</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="H2" s="44" t="s">
+        <v>234</v>
+      </c>
+      <c r="I2" s="39" t="str">
+        <f>_xlfn.CONCAT(D2:H2)</f>
+        <v>000000C350</v>
+      </c>
+      <c r="J2" s="39">
+        <f>HEX2DEC(I2)</f>
+        <v>50000</v>
+      </c>
+      <c r="K2" s="46">
+        <f>J2/1000</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="24">
+        <v>4</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="H3" s="44" t="s">
+        <v>236</v>
+      </c>
+      <c r="I3" s="39" t="str">
+        <f t="shared" ref="I3:I13" si="0">_xlfn.CONCAT(D3:H3)</f>
+        <v>00000007D0</v>
+      </c>
+      <c r="J3" s="39">
+        <f t="shared" ref="J3:J13" si="1">HEX2DEC(I3)</f>
+        <v>2000</v>
+      </c>
+      <c r="K3" s="46">
+        <f>J3/1000</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" s="24">
+        <v>4</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>228</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>237</v>
+      </c>
+      <c r="H4" s="44" t="s">
+        <v>238</v>
+      </c>
+      <c r="I4" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>00000186A0</v>
+      </c>
+      <c r="J4" s="39">
+        <f t="shared" si="1"/>
+        <v>100000</v>
+      </c>
+      <c r="K4" s="46">
+        <f>J4/1000</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C5" s="24">
+        <v>2</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="G5" s="26"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>0000FA</v>
+      </c>
+      <c r="J5" s="39">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="K5" s="47">
+        <f>INT(J5/10)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" s="24">
+        <v>2</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="G6" s="26"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>000032</v>
+      </c>
+      <c r="J6" s="39">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="K6" s="47">
+        <f>INT(J6/10)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C7" s="24">
+        <v>2</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="G7" s="26"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>000080</v>
+      </c>
+      <c r="J7" s="39">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="K7" s="47">
+        <f>INT(J7)</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C8" s="24">
+        <v>4</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>241</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="H8" s="44" t="s">
+        <v>243</v>
+      </c>
+      <c r="I8" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>003B9AA2F0</v>
+      </c>
+      <c r="J8" s="39">
+        <f t="shared" si="1"/>
+        <v>999990000</v>
+      </c>
+      <c r="K8" s="47">
+        <f>INT(J8-1000000000)</f>
+        <v>-10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C9" s="24">
+        <v>4</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>241</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="H9" s="44" t="s">
+        <v>207</v>
+      </c>
+      <c r="I9" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>003B9AF110</v>
+      </c>
+      <c r="J9" s="39">
+        <f t="shared" si="1"/>
+        <v>1000010000</v>
+      </c>
+      <c r="K9" s="47">
+        <f>INT(J9-1000000000)</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C10" s="24">
+        <v>4</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>241</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="H10" s="44" t="s">
+        <v>210</v>
+      </c>
+      <c r="I10" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>003B9ACA00</v>
+      </c>
+      <c r="J10" s="39">
+        <f t="shared" si="1"/>
+        <v>1000000000</v>
+      </c>
+      <c r="K10" s="47">
+        <f>INT(J10-1000000000)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C11" s="24">
+        <v>4</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>241</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="H11" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="I11" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>003B9AD9FF</v>
+      </c>
+      <c r="J11" s="39">
+        <f t="shared" si="1"/>
+        <v>1000004095</v>
+      </c>
+      <c r="K11" s="47">
+        <f>INT(J11-1000000000)</f>
+        <v>4095</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C12" s="24">
+        <v>4</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="H12" s="44" t="s">
+        <v>207</v>
+      </c>
+      <c r="I12" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>00000F4A10</v>
+      </c>
+      <c r="J12" s="39">
+        <f t="shared" si="1"/>
+        <v>1002000</v>
+      </c>
+      <c r="K12" s="48">
+        <f>(J12-1000000)/1000</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C13" s="24">
+        <v>4</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="G13" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="H13" s="44" t="s">
+        <v>213</v>
+      </c>
+      <c r="I13" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>00000F4240</v>
+      </c>
+      <c r="J13" s="39">
+        <f t="shared" si="1"/>
+        <v>1000000</v>
+      </c>
+      <c r="K13" s="46">
+        <f>(J13-1000000)/1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="C14" s="3">
+        <f>SUM(C2:C13)</f>
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added function to send current PID Setpoint value.
</commit_message>
<xml_diff>
--- a/Resources/DataPacket/Commands.xlsx
+++ b/Resources/DataPacket/Commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavi\Documents\Embed\STM32\Projects\CurrentController\Resources\DataPacket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A38085-32FD-49F6-89B0-A4930732163A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24CE209-0D90-4562-8FAC-8B62F6141EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23040" yWindow="108" windowWidth="23040" windowHeight="12228" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Packet" sheetId="4" r:id="rId1"/>
@@ -21,9 +21,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Commands v0.1'!$A$1:$K$29</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Commands v0.2'!$A$1:$K$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Commands v0.2'!$A$1:$K$16</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Commands v0.1'!$A$1:$K$18</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Commands v0.2'!$A$1:$K$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Commands v0.2'!$A$1:$K$15</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Data Packet'!$A$1:$F$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="254">
   <si>
     <t>Start byte 1</t>
   </si>
@@ -538,9 +538,6 @@
     <t>FREE</t>
   </si>
   <si>
-    <t>0x06 - 0x7F</t>
-  </si>
-  <si>
     <t>0x80</t>
   </si>
   <si>
@@ -809,14 +806,30 @@
   <si>
     <t>32</t>
   </si>
+  <si>
+    <t>0xAA 0x55 0x06 0x00 0xF9</t>
+  </si>
+  <si>
+    <t>0x06</t>
+  </si>
+  <si>
+    <t>0x07 - 0x7F</t>
+  </si>
+  <si>
+    <t>0xF9</t>
+  </si>
+  <si>
+    <t>Asks for the current PID Setpoint value (electrical current in mA):
+(4 bytes) = [0 : 4294967295] = [0x00000000 : 0xFFFFFFFF]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="#,##0.000"/>
-    <numFmt numFmtId="167" formatCode="#,##0.0"/>
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -1156,6 +1169,42 @@
     <xf numFmtId="49" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1184,42 +1233,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1524,14 +1537,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -2096,13 +2109,13 @@
       <c r="AG6" s="3"/>
     </row>
     <row r="7" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="29"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="41"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -2133,11 +2146,11 @@
       <c r="AG7" s="3"/>
     </row>
     <row r="8" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="32"/>
+      <c r="A8" s="42"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="44"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -2168,11 +2181,11 @@
       <c r="AG8" s="3"/>
     </row>
     <row r="9" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="32"/>
+      <c r="A9" s="42"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="44"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -2203,11 +2216,11 @@
       <c r="AG9" s="3"/>
     </row>
     <row r="10" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="32"/>
+      <c r="A10" s="42"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="44"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -2238,11 +2251,11 @@
       <c r="AG10" s="3"/>
     </row>
     <row r="11" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="32"/>
+      <c r="A11" s="42"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="44"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -2273,11 +2286,11 @@
       <c r="AG11" s="3"/>
     </row>
     <row r="12" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="32"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="44"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -2308,11 +2321,11 @@
       <c r="AG12" s="3"/>
     </row>
     <row r="13" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="32"/>
+      <c r="A13" s="42"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="44"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -2343,11 +2356,11 @@
       <c r="AG13" s="3"/>
     </row>
     <row r="14" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="32"/>
+      <c r="A14" s="42"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="44"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -2378,11 +2391,11 @@
       <c r="AG14" s="3"/>
     </row>
     <row r="15" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="32"/>
+      <c r="A15" s="42"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="44"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -2413,11 +2426,11 @@
       <c r="AG15" s="3"/>
     </row>
     <row r="16" spans="1:369" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="33"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="35"/>
+      <c r="A16" s="45"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="47"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -42750,10 +42763,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42905,7 +42918,7 @@
         <v>24</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K4" s="16" t="s">
         <v>18</v>
@@ -43086,82 +43099,82 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+    <row r="10" spans="1:11" s="18" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
         <v>9</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="K10" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C11" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D11" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="F10" s="12" t="s">
+      <c r="E11" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G11" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H11" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J11" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="K11" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="18" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
-        <v>10</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="J11" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="K11" s="16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="18" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="18" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>11</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>14</v>
@@ -43170,22 +43183,22 @@
         <v>15</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>120</v>
+        <v>161</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>55</v>
+        <v>143</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>53</v>
+        <v>144</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>50</v>
+        <v>165</v>
       </c>
       <c r="I12" s="16" t="s">
         <v>25</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="K12" s="16" t="s">
         <v>22</v>
@@ -43195,8 +43208,8 @@
       <c r="A13" s="16">
         <v>12</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>169</v>
+      <c r="B13" s="17" t="s">
+        <v>166</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>14</v>
@@ -43205,60 +43218,60 @@
         <v>15</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>168</v>
+        <v>120</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="17" t="s">
         <v>53</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>170</v>
+        <v>50</v>
       </c>
       <c r="I13" s="16" t="s">
         <v>25</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="K13" s="16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A14" s="12">
+    <row r="14" spans="1:11" s="18" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A14" s="16">
         <v>13</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I14" s="12" t="s">
+      <c r="B14" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="I14" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>18</v>
+      <c r="J14" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="K14" s="16" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -43266,7 +43279,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>18</v>
@@ -43275,7 +43288,7 @@
         <v>18</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>18</v>
@@ -43287,27 +43300,49 @@
         <v>18</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="K15" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="11"/>
+    <row r="16" spans="1:11" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A16" s="12">
+        <v>15</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
@@ -43335,8 +43370,21 @@
       <c r="J18" s="14"/>
       <c r="K18" s="11"/>
     </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="11"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K15" xr:uid="{B11DB8B0-5B17-4A82-8032-D4706BCA4450}"/>
+  <autoFilter ref="A1:K16" xr:uid="{B11DB8B0-5B17-4A82-8032-D4706BCA4450}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup scale="39" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
@@ -43355,11 +43403,11 @@
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="2" width="28.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" style="41" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" style="31" customWidth="1"/>
     <col min="5" max="8" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.140625" style="3" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="17" style="37" customWidth="1"/>
+    <col min="11" max="11" width="17" style="27" customWidth="1"/>
     <col min="12" max="18" width="9.140625" style="3"/>
   </cols>
   <sheetData>
@@ -43368,34 +43416,34 @@
         <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="D1" s="40" t="s">
-        <v>221</v>
+        <v>180</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>220</v>
       </c>
       <c r="E1" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="F1" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="G1" s="25" t="s">
         <v>193</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="H1" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="I1" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="J1" s="28" t="s">
         <v>196</v>
       </c>
-      <c r="J1" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="K1" s="45" t="s">
-        <v>219</v>
+      <c r="K1" s="35" t="s">
+        <v>218</v>
       </c>
       <c r="L1" s="22"/>
       <c r="M1" s="22"/>
@@ -43410,35 +43458,35 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C2" s="24">
         <v>4</v>
       </c>
-      <c r="D2" s="42" t="s">
-        <v>210</v>
+      <c r="D2" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F2" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G2" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="H2" s="44" t="s">
-        <v>191</v>
-      </c>
-      <c r="I2" s="39" t="str">
+        <v>221</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="I2" s="29" t="str">
         <f>_xlfn.CONCAT(D2:H2)</f>
         <v>00000085f1</v>
       </c>
-      <c r="J2" s="39">
+      <c r="J2" s="29">
         <f>HEX2DEC(I2)</f>
         <v>34289</v>
       </c>
-      <c r="K2" s="46">
+      <c r="K2" s="36">
         <f>J2/1000</f>
         <v>34.289000000000001</v>
       </c>
@@ -43448,35 +43496,35 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C3" s="24">
         <v>4</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="G3" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="E3" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="G3" s="26" t="s">
-        <v>211</v>
-      </c>
-      <c r="H3" s="44" t="s">
-        <v>224</v>
-      </c>
-      <c r="I3" s="39" t="str">
+      <c r="H3" s="34" t="s">
+        <v>223</v>
+      </c>
+      <c r="I3" s="29" t="str">
         <f t="shared" ref="I3:I13" si="0">_xlfn.CONCAT(D3:H3)</f>
         <v>000000ea48</v>
       </c>
-      <c r="J3" s="39">
+      <c r="J3" s="29">
         <f t="shared" ref="J3:J13" si="1">HEX2DEC(I3)</f>
         <v>59976</v>
       </c>
-      <c r="K3" s="46">
+      <c r="K3" s="36">
         <f>J3/1000</f>
         <v>59.975999999999999</v>
       </c>
@@ -43486,35 +43534,35 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C4" s="24">
         <v>4</v>
       </c>
-      <c r="D4" s="42" t="s">
-        <v>210</v>
+      <c r="D4" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G4" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="H4" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="H4" s="44" t="s">
-        <v>226</v>
-      </c>
-      <c r="I4" s="39" t="str">
+      <c r="I4" s="29" t="str">
         <f t="shared" si="0"/>
         <v>00000079ed</v>
       </c>
-      <c r="J4" s="39">
+      <c r="J4" s="29">
         <f t="shared" si="1"/>
         <v>31213</v>
       </c>
-      <c r="K4" s="46">
+      <c r="K4" s="36">
         <f>J4/1000</f>
         <v>31.213000000000001</v>
       </c>
@@ -43524,31 +43572,31 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C5" s="24">
         <v>2</v>
       </c>
-      <c r="D5" s="42" t="s">
-        <v>210</v>
+      <c r="D5" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G5" s="26"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="39" t="str">
+      <c r="H5" s="34"/>
+      <c r="I5" s="29" t="str">
         <f t="shared" si="0"/>
         <v>001546</v>
       </c>
-      <c r="J5" s="39">
+      <c r="J5" s="29">
         <f t="shared" si="1"/>
         <v>5446</v>
       </c>
-      <c r="K5" s="47">
+      <c r="K5" s="37">
         <f>INT(J5/10)</f>
         <v>544</v>
       </c>
@@ -43558,31 +43606,31 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C6" s="24">
         <v>2</v>
       </c>
-      <c r="D6" s="42" t="s">
-        <v>210</v>
+      <c r="D6" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F6" s="26" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G6" s="26"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="39" t="str">
+      <c r="H6" s="34"/>
+      <c r="I6" s="29" t="str">
         <f t="shared" si="0"/>
         <v>00adbc</v>
       </c>
-      <c r="J6" s="39">
+      <c r="J6" s="29">
         <f t="shared" si="1"/>
         <v>44476</v>
       </c>
-      <c r="K6" s="47">
+      <c r="K6" s="37">
         <f>INT(J6/10)</f>
         <v>4447</v>
       </c>
@@ -43592,31 +43640,31 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C7" s="24">
         <v>2</v>
       </c>
-      <c r="D7" s="42" t="s">
-        <v>210</v>
+      <c r="D7" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="E7" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="F7" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="F7" s="26" t="s">
-        <v>202</v>
-      </c>
       <c r="G7" s="26"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="39" t="str">
+      <c r="H7" s="34"/>
+      <c r="I7" s="29" t="str">
         <f t="shared" si="0"/>
         <v>002143</v>
       </c>
-      <c r="J7" s="39">
+      <c r="J7" s="29">
         <f t="shared" si="1"/>
         <v>8515</v>
       </c>
-      <c r="K7" s="47">
+      <c r="K7" s="37">
         <f>INT(J7)</f>
         <v>8515</v>
       </c>
@@ -43626,35 +43674,35 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C8" s="24">
         <v>4</v>
       </c>
-      <c r="D8" s="42" t="s">
-        <v>210</v>
+      <c r="D8" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F8" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="G8" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="H8" s="34" t="s">
         <v>205</v>
       </c>
-      <c r="H8" s="44" t="s">
-        <v>206</v>
-      </c>
-      <c r="I8" s="39" t="str">
+      <c r="I8" s="29" t="str">
         <f t="shared" si="0"/>
         <v>0000e0ff54</v>
       </c>
-      <c r="J8" s="39">
+      <c r="J8" s="29">
         <f t="shared" si="1"/>
         <v>14745428</v>
       </c>
-      <c r="K8" s="47">
+      <c r="K8" s="37">
         <f>INT(J8-1000000000)</f>
         <v>-985254572</v>
       </c>
@@ -43664,35 +43712,35 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C9" s="24">
         <v>4</v>
       </c>
-      <c r="D9" s="42" t="s">
-        <v>210</v>
+      <c r="D9" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G9" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="H9" s="44" t="s">
-        <v>207</v>
-      </c>
-      <c r="I9" s="39" t="str">
+        <v>228</v>
+      </c>
+      <c r="H9" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="I9" s="29" t="str">
         <f t="shared" si="0"/>
         <v>006a052010</v>
       </c>
-      <c r="J9" s="39">
+      <c r="J9" s="29">
         <f t="shared" si="1"/>
         <v>1778720784</v>
       </c>
-      <c r="K9" s="47">
+      <c r="K9" s="37">
         <f>INT(J9-1000000000)</f>
         <v>778720784</v>
       </c>
@@ -43702,35 +43750,35 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C10" s="24">
         <v>4</v>
       </c>
-      <c r="D10" s="42" t="s">
-        <v>210</v>
+      <c r="D10" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F10" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="G10" s="26" t="s">
         <v>208</v>
       </c>
-      <c r="G10" s="26" t="s">
+      <c r="H10" s="34" t="s">
         <v>209</v>
       </c>
-      <c r="H10" s="44" t="s">
-        <v>210</v>
-      </c>
-      <c r="I10" s="39" t="str">
+      <c r="I10" s="29" t="str">
         <f t="shared" si="0"/>
         <v>0064980200</v>
       </c>
-      <c r="J10" s="39">
+      <c r="J10" s="29">
         <f t="shared" si="1"/>
         <v>1687683584</v>
       </c>
-      <c r="K10" s="47">
+      <c r="K10" s="37">
         <f>INT(J10-1000000000)</f>
         <v>687683584</v>
       </c>
@@ -43740,35 +43788,35 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C11" s="24">
         <v>4</v>
       </c>
-      <c r="D11" s="42" t="s">
-        <v>210</v>
+      <c r="D11" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F11" s="26" t="s">
+        <v>211</v>
+      </c>
+      <c r="G11" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="G11" s="26" t="s">
+      <c r="H11" s="34" t="s">
         <v>213</v>
       </c>
-      <c r="H11" s="44" t="s">
-        <v>214</v>
-      </c>
-      <c r="I11" s="39" t="str">
+      <c r="I11" s="29" t="str">
         <f t="shared" si="0"/>
         <v>002bae4080</v>
       </c>
-      <c r="J11" s="39">
+      <c r="J11" s="29">
         <f t="shared" si="1"/>
         <v>732840064</v>
       </c>
-      <c r="K11" s="47">
+      <c r="K11" s="37">
         <f>INT(J11-1000000000)</f>
         <v>-267159936</v>
       </c>
@@ -43778,35 +43826,35 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C12" s="24">
         <v>4</v>
       </c>
-      <c r="D12" s="42" t="s">
-        <v>210</v>
+      <c r="D12" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F12" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="G12" s="26" t="s">
         <v>215</v>
       </c>
-      <c r="G12" s="26" t="s">
+      <c r="H12" s="34" t="s">
         <v>216</v>
       </c>
-      <c r="H12" s="44" t="s">
-        <v>217</v>
-      </c>
-      <c r="I12" s="39" t="str">
+      <c r="I12" s="29" t="str">
         <f t="shared" si="0"/>
         <v>002812eeab</v>
       </c>
-      <c r="J12" s="39">
+      <c r="J12" s="29">
         <f t="shared" si="1"/>
         <v>672329387</v>
       </c>
-      <c r="K12" s="48">
+      <c r="K12" s="38">
         <f>(J12-1000000)/1000</f>
         <v>671329.38699999999</v>
       </c>
@@ -43816,42 +43864,42 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C13" s="24">
         <v>4</v>
       </c>
-      <c r="D13" s="42" t="s">
-        <v>210</v>
+      <c r="D13" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="H13" s="44" t="s">
-        <v>218</v>
-      </c>
-      <c r="I13" s="39" t="str">
+        <v>209</v>
+      </c>
+      <c r="H13" s="34" t="s">
+        <v>217</v>
+      </c>
+      <c r="I13" s="29" t="str">
         <f t="shared" si="0"/>
         <v>0000000056</v>
       </c>
-      <c r="J13" s="39">
+      <c r="J13" s="29">
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
-      <c r="K13" s="46">
+      <c r="K13" s="36">
         <f>(J13-1000000)/1000</f>
         <v>-999.91399999999999</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C14" s="3">
         <f>SUM(C2:C13)</f>
@@ -43867,7 +43915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F1C60FF-9CA3-4972-9764-D5189C56A132}">
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
@@ -43876,11 +43924,11 @@
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="2" width="28.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" style="41" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" style="31" customWidth="1"/>
     <col min="5" max="8" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.140625" style="3" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="17" style="37" customWidth="1"/>
+    <col min="11" max="11" width="17" style="27" customWidth="1"/>
     <col min="12" max="18" width="9.140625" style="3"/>
   </cols>
   <sheetData>
@@ -43889,34 +43937,34 @@
         <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="D1" s="40" t="s">
-        <v>221</v>
+        <v>180</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>220</v>
       </c>
       <c r="E1" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="F1" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="G1" s="25" t="s">
         <v>193</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="H1" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="I1" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="J1" s="28" t="s">
         <v>196</v>
       </c>
-      <c r="J1" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="K1" s="45" t="s">
-        <v>219</v>
+      <c r="K1" s="35" t="s">
+        <v>218</v>
       </c>
       <c r="L1" s="22"/>
       <c r="M1" s="22"/>
@@ -43931,35 +43979,35 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C2" s="24">
         <v>4</v>
       </c>
-      <c r="D2" s="42" t="s">
-        <v>210</v>
+      <c r="D2" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F2" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G2" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="H2" s="34" t="s">
         <v>233</v>
       </c>
-      <c r="H2" s="44" t="s">
-        <v>234</v>
-      </c>
-      <c r="I2" s="39" t="str">
+      <c r="I2" s="29" t="str">
         <f>_xlfn.CONCAT(D2:H2)</f>
         <v>000000C350</v>
       </c>
-      <c r="J2" s="39">
+      <c r="J2" s="29">
         <f>HEX2DEC(I2)</f>
         <v>50000</v>
       </c>
-      <c r="K2" s="46">
+      <c r="K2" s="36">
         <f>J2/1000</f>
         <v>50</v>
       </c>
@@ -43969,35 +44017,35 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C3" s="24">
         <v>4</v>
       </c>
-      <c r="D3" s="42" t="s">
-        <v>210</v>
+      <c r="D3" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F3" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G3" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="H3" s="34" t="s">
         <v>235</v>
       </c>
-      <c r="H3" s="44" t="s">
-        <v>236</v>
-      </c>
-      <c r="I3" s="39" t="str">
+      <c r="I3" s="29" t="str">
         <f t="shared" ref="I3:I13" si="0">_xlfn.CONCAT(D3:H3)</f>
         <v>00000007D0</v>
       </c>
-      <c r="J3" s="39">
+      <c r="J3" s="29">
         <f t="shared" ref="J3:J13" si="1">HEX2DEC(I3)</f>
         <v>2000</v>
       </c>
-      <c r="K3" s="46">
+      <c r="K3" s="36">
         <f>J3/1000</f>
         <v>2</v>
       </c>
@@ -44007,35 +44055,35 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C4" s="24">
         <v>4</v>
       </c>
-      <c r="D4" s="42" t="s">
-        <v>210</v>
+      <c r="D4" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G4" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="H4" s="34" t="s">
         <v>237</v>
       </c>
-      <c r="H4" s="44" t="s">
-        <v>238</v>
-      </c>
-      <c r="I4" s="39" t="str">
+      <c r="I4" s="29" t="str">
         <f t="shared" si="0"/>
         <v>00000186A0</v>
       </c>
-      <c r="J4" s="39">
+      <c r="J4" s="29">
         <f t="shared" si="1"/>
         <v>100000</v>
       </c>
-      <c r="K4" s="46">
+      <c r="K4" s="36">
         <f>J4/1000</f>
         <v>100</v>
       </c>
@@ -44045,31 +44093,31 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C5" s="24">
         <v>2</v>
       </c>
-      <c r="D5" s="42" t="s">
-        <v>210</v>
+      <c r="D5" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G5" s="26"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="39" t="str">
+      <c r="H5" s="34"/>
+      <c r="I5" s="29" t="str">
         <f t="shared" si="0"/>
         <v>0000FA</v>
       </c>
-      <c r="J5" s="39">
+      <c r="J5" s="29">
         <f t="shared" si="1"/>
         <v>250</v>
       </c>
-      <c r="K5" s="47">
+      <c r="K5" s="37">
         <f>INT(J5/10)</f>
         <v>25</v>
       </c>
@@ -44079,31 +44127,31 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C6" s="24">
         <v>2</v>
       </c>
-      <c r="D6" s="42" t="s">
-        <v>210</v>
+      <c r="D6" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F6" s="26" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G6" s="26"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="39" t="str">
+      <c r="H6" s="34"/>
+      <c r="I6" s="29" t="str">
         <f t="shared" si="0"/>
         <v>000032</v>
       </c>
-      <c r="J6" s="39">
+      <c r="J6" s="29">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="K6" s="47">
+      <c r="K6" s="37">
         <f>INT(J6/10)</f>
         <v>5</v>
       </c>
@@ -44113,31 +44161,31 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C7" s="24">
         <v>2</v>
       </c>
-      <c r="D7" s="42" t="s">
-        <v>210</v>
+      <c r="D7" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G7" s="26"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="39" t="str">
+      <c r="H7" s="34"/>
+      <c r="I7" s="29" t="str">
         <f t="shared" si="0"/>
         <v>000080</v>
       </c>
-      <c r="J7" s="39">
+      <c r="J7" s="29">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
-      <c r="K7" s="47">
+      <c r="K7" s="37">
         <f>INT(J7)</f>
         <v>128</v>
       </c>
@@ -44147,35 +44195,35 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C8" s="24">
         <v>4</v>
       </c>
-      <c r="D8" s="42" t="s">
-        <v>210</v>
+      <c r="D8" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="E8" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="F8" s="26" t="s">
         <v>240</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="G8" s="26" t="s">
         <v>241</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="H8" s="34" t="s">
         <v>242</v>
       </c>
-      <c r="H8" s="44" t="s">
-        <v>243</v>
-      </c>
-      <c r="I8" s="39" t="str">
+      <c r="I8" s="29" t="str">
         <f t="shared" si="0"/>
         <v>003B9AA2F0</v>
       </c>
-      <c r="J8" s="39">
+      <c r="J8" s="29">
         <f t="shared" si="1"/>
         <v>999990000</v>
       </c>
-      <c r="K8" s="47">
+      <c r="K8" s="37">
         <f>INT(J8-1000000000)</f>
         <v>-10000</v>
       </c>
@@ -44185,35 +44233,35 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C9" s="24">
         <v>4</v>
       </c>
-      <c r="D9" s="42" t="s">
-        <v>210</v>
+      <c r="D9" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="E9" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="F9" s="26" t="s">
         <v>240</v>
       </c>
-      <c r="F9" s="26" t="s">
-        <v>241</v>
-      </c>
       <c r="G9" s="26" t="s">
-        <v>244</v>
-      </c>
-      <c r="H9" s="44" t="s">
-        <v>207</v>
-      </c>
-      <c r="I9" s="39" t="str">
+        <v>243</v>
+      </c>
+      <c r="H9" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="I9" s="29" t="str">
         <f t="shared" si="0"/>
         <v>003B9AF110</v>
       </c>
-      <c r="J9" s="39">
+      <c r="J9" s="29">
         <f t="shared" si="1"/>
         <v>1000010000</v>
       </c>
-      <c r="K9" s="47">
+      <c r="K9" s="37">
         <f>INT(J9-1000000000)</f>
         <v>10000</v>
       </c>
@@ -44223,35 +44271,35 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C10" s="24">
         <v>4</v>
       </c>
-      <c r="D10" s="42" t="s">
-        <v>210</v>
+      <c r="D10" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="E10" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="F10" s="26" t="s">
         <v>240</v>
       </c>
-      <c r="F10" s="26" t="s">
-        <v>241</v>
-      </c>
       <c r="G10" s="26" t="s">
-        <v>245</v>
-      </c>
-      <c r="H10" s="44" t="s">
-        <v>210</v>
-      </c>
-      <c r="I10" s="39" t="str">
+        <v>244</v>
+      </c>
+      <c r="H10" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="I10" s="29" t="str">
         <f t="shared" si="0"/>
         <v>003B9ACA00</v>
       </c>
-      <c r="J10" s="39">
+      <c r="J10" s="29">
         <f t="shared" si="1"/>
         <v>1000000000</v>
       </c>
-      <c r="K10" s="47">
+      <c r="K10" s="37">
         <f>INT(J10-1000000000)</f>
         <v>0</v>
       </c>
@@ -44261,35 +44309,35 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C11" s="24">
         <v>4</v>
       </c>
-      <c r="D11" s="42" t="s">
-        <v>210</v>
+      <c r="D11" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="E11" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="F11" s="26" t="s">
         <v>240</v>
       </c>
-      <c r="F11" s="26" t="s">
-        <v>241</v>
-      </c>
       <c r="G11" s="26" t="s">
-        <v>246</v>
-      </c>
-      <c r="H11" s="44" t="s">
-        <v>220</v>
-      </c>
-      <c r="I11" s="39" t="str">
+        <v>245</v>
+      </c>
+      <c r="H11" s="34" t="s">
+        <v>219</v>
+      </c>
+      <c r="I11" s="29" t="str">
         <f t="shared" si="0"/>
         <v>003B9AD9FF</v>
       </c>
-      <c r="J11" s="39">
+      <c r="J11" s="29">
         <f t="shared" si="1"/>
         <v>1000004095</v>
       </c>
-      <c r="K11" s="47">
+      <c r="K11" s="37">
         <f>INT(J11-1000000000)</f>
         <v>4095</v>
       </c>
@@ -44299,35 +44347,35 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C12" s="24">
         <v>4</v>
       </c>
-      <c r="D12" s="42" t="s">
-        <v>210</v>
+      <c r="D12" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F12" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="G12" s="26" t="s">
         <v>247</v>
       </c>
-      <c r="G12" s="26" t="s">
-        <v>248</v>
-      </c>
-      <c r="H12" s="44" t="s">
-        <v>207</v>
-      </c>
-      <c r="I12" s="39" t="str">
+      <c r="H12" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="I12" s="29" t="str">
         <f t="shared" si="0"/>
         <v>00000F4A10</v>
       </c>
-      <c r="J12" s="39">
+      <c r="J12" s="29">
         <f t="shared" si="1"/>
         <v>1002000</v>
       </c>
-      <c r="K12" s="48">
+      <c r="K12" s="38">
         <f>(J12-1000000)/1000</f>
         <v>2</v>
       </c>
@@ -44337,42 +44385,42 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C13" s="24">
         <v>4</v>
       </c>
-      <c r="D13" s="42" t="s">
-        <v>210</v>
+      <c r="D13" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="H13" s="44" t="s">
-        <v>213</v>
-      </c>
-      <c r="I13" s="39" t="str">
+        <v>222</v>
+      </c>
+      <c r="H13" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="I13" s="29" t="str">
         <f t="shared" si="0"/>
         <v>00000F4240</v>
       </c>
-      <c r="J13" s="39">
+      <c r="J13" s="29">
         <f t="shared" si="1"/>
         <v>1000000</v>
       </c>
-      <c r="K13" s="46">
+      <c r="K13" s="36">
         <f>(J13-1000000)/1000</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C14" s="3">
         <f>SUM(C2:C13)</f>

</xml_diff>

<commit_message>
Added functionality of send keep alive message through serial communication with PID controller status.
</commit_message>
<xml_diff>
--- a/Resources/DataPacket/Commands.xlsx
+++ b/Resources/DataPacket/Commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavi\Documents\Embed\STM32\Projects\CurrentController\Resources\DataPacket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24CE209-0D90-4562-8FAC-8B62F6141EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D28A04D-A77A-4C56-8D62-FA1553B93AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23040" yWindow="108" windowWidth="23040" windowHeight="12228" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Packet" sheetId="4" r:id="rId1"/>
@@ -21,9 +21,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Commands v0.1'!$A$1:$K$29</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Commands v0.2'!$A$1:$K$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Commands v0.2'!$A$1:$K$17</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Commands v0.1'!$A$1:$K$18</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Commands v0.2'!$A$1:$K$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Commands v0.2'!$A$1:$K$16</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Data Packet'!$A$1:$F$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="258">
   <si>
     <t>Start byte 1</t>
   </si>
@@ -571,9 +571,6 @@
 (4 byter) = [0 : 4294967295] = [0x00000000 : 0xFFFFFFFF]</t>
   </si>
   <si>
-    <t>0x83 - 0xFE</t>
-  </si>
-  <si>
     <t>0XFF</t>
   </si>
   <si>
@@ -821,6 +818,21 @@
   <si>
     <t>Asks for the current PID Setpoint value (electrical current in mA):
 (4 bytes) = [0 : 4294967295] = [0x00000000 : 0xFFFFFFFF]</t>
+  </si>
+  <si>
+    <t>0xAA 0x55 0x83 0x01 0x00 0x3F</t>
+  </si>
+  <si>
+    <t>0x83</t>
+  </si>
+  <si>
+    <t>0x84 - 0xFE</t>
+  </si>
+  <si>
+    <t>0x3F</t>
+  </si>
+  <si>
+    <t>Send a keep alive message with status of PID Controller</t>
   </si>
 </sst>
 </file>
@@ -42763,10 +42775,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43104,7 +43116,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>14</v>
@@ -43113,7 +43125,7 @@
         <v>15</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>17</v>
@@ -43122,13 +43134,13 @@
         <v>18</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I10" s="16" t="s">
         <v>24</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K10" s="16" t="s">
         <v>18</v>
@@ -43148,7 +43160,7 @@
         <v>18</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>18</v>
@@ -43233,7 +43245,7 @@
         <v>25</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K13" s="16" t="s">
         <v>22</v>
@@ -43274,39 +43286,39 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A15" s="12">
+    <row r="15" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
         <v>14</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" s="12" t="s">
+      <c r="B15" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="I15" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="J15" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="K15" s="12" t="s">
-        <v>18</v>
+      <c r="J15" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="K15" s="16" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -43314,7 +43326,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>18</v>
@@ -43323,7 +43335,7 @@
         <v>18</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>172</v>
+        <v>255</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>18</v>
@@ -43335,27 +43347,49 @@
         <v>18</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="K16" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="11"/>
+    <row r="17" spans="1:11" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A17" s="12">
+        <v>16</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
@@ -43383,8 +43417,21 @@
       <c r="J19" s="14"/>
       <c r="K19" s="11"/>
     </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="11"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K16" xr:uid="{B11DB8B0-5B17-4A82-8032-D4706BCA4450}"/>
+  <autoFilter ref="A1:K17" xr:uid="{B11DB8B0-5B17-4A82-8032-D4706BCA4450}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup scale="39" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
@@ -43416,34 +43463,34 @@
         <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E1" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="F1" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="G1" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="H1" s="33" t="s">
         <v>193</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="I1" s="28" t="s">
         <v>194</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="J1" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="J1" s="28" t="s">
-        <v>196</v>
-      </c>
       <c r="K1" s="35" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L1" s="22"/>
       <c r="M1" s="22"/>
@@ -43458,25 +43505,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C2" s="24">
         <v>4</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F2" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G2" s="26" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I2" s="29" t="str">
         <f>_xlfn.CONCAT(D2:H2)</f>
@@ -43496,25 +43543,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C3" s="24">
         <v>4</v>
       </c>
       <c r="D3" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="G3" s="26" t="s">
         <v>209</v>
       </c>
-      <c r="E3" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="G3" s="26" t="s">
-        <v>210</v>
-      </c>
       <c r="H3" s="34" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I3" s="29" t="str">
         <f t="shared" ref="I3:I13" si="0">_xlfn.CONCAT(D3:H3)</f>
@@ -43534,25 +43581,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C4" s="24">
         <v>4</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G4" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="H4" s="34" t="s">
         <v>224</v>
-      </c>
-      <c r="H4" s="34" t="s">
-        <v>225</v>
       </c>
       <c r="I4" s="29" t="str">
         <f t="shared" si="0"/>
@@ -43572,19 +43619,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C5" s="24">
         <v>2</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G5" s="26"/>
       <c r="H5" s="34"/>
@@ -43606,19 +43653,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C6" s="24">
         <v>2</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F6" s="26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G6" s="26"/>
       <c r="H6" s="34"/>
@@ -43640,19 +43687,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C7" s="24">
         <v>2</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E7" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="F7" s="26" t="s">
         <v>200</v>
-      </c>
-      <c r="F7" s="26" t="s">
-        <v>201</v>
       </c>
       <c r="G7" s="26"/>
       <c r="H7" s="34"/>
@@ -43674,25 +43721,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C8" s="24">
         <v>4</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F8" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="G8" s="26" t="s">
         <v>203</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="H8" s="34" t="s">
         <v>204</v>
-      </c>
-      <c r="H8" s="34" t="s">
-        <v>205</v>
       </c>
       <c r="I8" s="29" t="str">
         <f t="shared" si="0"/>
@@ -43712,25 +43759,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C9" s="24">
         <v>4</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G9" s="26" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H9" s="34" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I9" s="29" t="str">
         <f t="shared" si="0"/>
@@ -43750,25 +43797,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C10" s="24">
         <v>4</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F10" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="G10" s="26" t="s">
         <v>207</v>
       </c>
-      <c r="G10" s="26" t="s">
+      <c r="H10" s="34" t="s">
         <v>208</v>
-      </c>
-      <c r="H10" s="34" t="s">
-        <v>209</v>
       </c>
       <c r="I10" s="29" t="str">
         <f t="shared" si="0"/>
@@ -43788,25 +43835,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C11" s="24">
         <v>4</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F11" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="G11" s="26" t="s">
         <v>211</v>
       </c>
-      <c r="G11" s="26" t="s">
+      <c r="H11" s="34" t="s">
         <v>212</v>
-      </c>
-      <c r="H11" s="34" t="s">
-        <v>213</v>
       </c>
       <c r="I11" s="29" t="str">
         <f t="shared" si="0"/>
@@ -43826,25 +43873,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C12" s="24">
         <v>4</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F12" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="G12" s="26" t="s">
         <v>214</v>
       </c>
-      <c r="G12" s="26" t="s">
+      <c r="H12" s="34" t="s">
         <v>215</v>
-      </c>
-      <c r="H12" s="34" t="s">
-        <v>216</v>
       </c>
       <c r="I12" s="29" t="str">
         <f t="shared" si="0"/>
@@ -43864,25 +43911,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C13" s="24">
         <v>4</v>
       </c>
       <c r="D13" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H13" s="34" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I13" s="29" t="str">
         <f t="shared" si="0"/>
@@ -43899,7 +43946,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C14" s="3">
         <f>SUM(C2:C13)</f>
@@ -43937,34 +43984,34 @@
         <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E1" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="F1" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="G1" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="H1" s="33" t="s">
         <v>193</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="I1" s="28" t="s">
         <v>194</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="J1" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="J1" s="28" t="s">
-        <v>196</v>
-      </c>
       <c r="K1" s="35" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L1" s="22"/>
       <c r="M1" s="22"/>
@@ -43979,25 +44026,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C2" s="24">
         <v>4</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F2" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G2" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="H2" s="34" t="s">
         <v>232</v>
-      </c>
-      <c r="H2" s="34" t="s">
-        <v>233</v>
       </c>
       <c r="I2" s="29" t="str">
         <f>_xlfn.CONCAT(D2:H2)</f>
@@ -44017,25 +44064,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C3" s="24">
         <v>4</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F3" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G3" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="H3" s="34" t="s">
         <v>234</v>
-      </c>
-      <c r="H3" s="34" t="s">
-        <v>235</v>
       </c>
       <c r="I3" s="29" t="str">
         <f t="shared" ref="I3:I13" si="0">_xlfn.CONCAT(D3:H3)</f>
@@ -44055,25 +44102,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C4" s="24">
         <v>4</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G4" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="H4" s="34" t="s">
         <v>236</v>
-      </c>
-      <c r="H4" s="34" t="s">
-        <v>237</v>
       </c>
       <c r="I4" s="29" t="str">
         <f t="shared" si="0"/>
@@ -44093,19 +44140,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C5" s="24">
         <v>2</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G5" s="26"/>
       <c r="H5" s="34"/>
@@ -44127,19 +44174,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C6" s="24">
         <v>2</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F6" s="26" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G6" s="26"/>
       <c r="H6" s="34"/>
@@ -44161,19 +44208,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C7" s="24">
         <v>2</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G7" s="26"/>
       <c r="H7" s="34"/>
@@ -44195,25 +44242,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C8" s="24">
         <v>4</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E8" s="26" t="s">
+        <v>238</v>
+      </c>
+      <c r="F8" s="26" t="s">
         <v>239</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="G8" s="26" t="s">
         <v>240</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="H8" s="34" t="s">
         <v>241</v>
-      </c>
-      <c r="H8" s="34" t="s">
-        <v>242</v>
       </c>
       <c r="I8" s="29" t="str">
         <f t="shared" si="0"/>
@@ -44233,25 +44280,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C9" s="24">
         <v>4</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E9" s="26" t="s">
+        <v>238</v>
+      </c>
+      <c r="F9" s="26" t="s">
         <v>239</v>
       </c>
-      <c r="F9" s="26" t="s">
-        <v>240</v>
-      </c>
       <c r="G9" s="26" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H9" s="34" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I9" s="29" t="str">
         <f t="shared" si="0"/>
@@ -44271,25 +44318,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C10" s="24">
         <v>4</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E10" s="26" t="s">
+        <v>238</v>
+      </c>
+      <c r="F10" s="26" t="s">
         <v>239</v>
       </c>
-      <c r="F10" s="26" t="s">
-        <v>240</v>
-      </c>
       <c r="G10" s="26" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H10" s="34" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I10" s="29" t="str">
         <f t="shared" si="0"/>
@@ -44309,25 +44356,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C11" s="24">
         <v>4</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E11" s="26" t="s">
+        <v>238</v>
+      </c>
+      <c r="F11" s="26" t="s">
         <v>239</v>
       </c>
-      <c r="F11" s="26" t="s">
-        <v>240</v>
-      </c>
       <c r="G11" s="26" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H11" s="34" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I11" s="29" t="str">
         <f t="shared" si="0"/>
@@ -44347,25 +44394,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C12" s="24">
         <v>4</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F12" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="G12" s="26" t="s">
         <v>246</v>
       </c>
-      <c r="G12" s="26" t="s">
-        <v>247</v>
-      </c>
       <c r="H12" s="34" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I12" s="29" t="str">
         <f t="shared" si="0"/>
@@ -44385,25 +44432,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C13" s="24">
         <v>4</v>
       </c>
       <c r="D13" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H13" s="34" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I13" s="29" t="str">
         <f t="shared" si="0"/>
@@ -44420,7 +44467,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C14" s="3">
         <f>SUM(C2:C13)</f>

</xml_diff>

<commit_message>
Changed the controller default values (pid and sampling time).
</commit_message>
<xml_diff>
--- a/Resources/DataPacket/Commands.xlsx
+++ b/Resources/DataPacket/Commands.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavi\Documents\Embed\STM32\Projects\CurrentController\Resources\DataPacket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D28A04D-A77A-4C56-8D62-FA1553B93AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23905152-E5B6-467E-AD68-48036499AF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Packet" sheetId="4" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Commands v0.2" sheetId="6" r:id="rId3"/>
     <sheet name="Config data" sheetId="7" r:id="rId4"/>
     <sheet name="Config data (2)" sheetId="8" r:id="rId5"/>
+    <sheet name="Config data (3)" sheetId="9" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Commands v0.1'!$A$1:$K$29</definedName>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="276">
   <si>
     <t>Start byte 1</t>
   </si>
@@ -834,6 +835,60 @@
   <si>
     <t>Send a keep alive message with status of PID Controller</t>
   </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>2a</t>
+  </si>
+  <si>
+    <t>c3</t>
+  </si>
+  <si>
+    <t>0b</t>
+  </si>
+  <si>
+    <t>b8</t>
+  </si>
+  <si>
+    <t>a0</t>
+  </si>
+  <si>
+    <t>fa</t>
+  </si>
+  <si>
+    <t>3b</t>
+  </si>
+  <si>
+    <t>9a</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>f0</t>
+  </si>
+  <si>
+    <t>ca</t>
+  </si>
+  <si>
+    <t>d9</t>
+  </si>
+  <si>
+    <t>0f</t>
+  </si>
+  <si>
+    <t>4a</t>
+  </si>
+  <si>
+    <t>PC -&gt; UC</t>
+  </si>
+  <si>
+    <t>7d</t>
+  </si>
+  <si>
+    <t>d0</t>
+  </si>
 </sst>
 </file>
 
@@ -920,7 +975,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1103,11 +1158,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1247,6 +1315,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -42777,7 +42869,7 @@
   </sheetPr>
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -44477,4 +44569,1465 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4CEB2E4-46E8-427F-8D2D-4ACA4FDFFF40}">
+  <dimension ref="A1:BG31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="28.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" style="31" customWidth="1"/>
+    <col min="5" max="8" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="17" style="27" customWidth="1"/>
+    <col min="12" max="16" width="4.140625" style="3" customWidth="1"/>
+    <col min="17" max="18" width="3" style="31" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="2.85546875" style="51" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="3" style="51" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="3.140625" style="51" bestFit="1" customWidth="1"/>
+    <col min="25" max="29" width="3" style="51" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="2.7109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="31" max="34" width="3" style="51" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="3.140625" style="51" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="3" style="51" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="2.7109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="3.140625" style="51" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="3" style="51" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="2.7109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="3" style="51" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="3.140625" style="51" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="3" style="51" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="2.85546875" style="51" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="3" style="51" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="3.140625" style="51" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="3" style="51" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="3.140625" style="51" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="2.42578125" style="51" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="3" style="51" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="2.7109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="53" max="55" width="3" style="51" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="2.7109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="57" max="58" width="3" style="51" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:59" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="K1" s="35" t="s">
+        <v>217</v>
+      </c>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="50"/>
+      <c r="AA1" s="50"/>
+      <c r="AB1" s="50"/>
+      <c r="AC1" s="50"/>
+      <c r="AD1" s="50"/>
+      <c r="AE1" s="50"/>
+      <c r="AF1" s="50"/>
+      <c r="AG1" s="50"/>
+      <c r="AH1" s="50"/>
+      <c r="AI1" s="50"/>
+      <c r="AJ1" s="50"/>
+      <c r="AK1" s="50"/>
+      <c r="AL1" s="50"/>
+      <c r="AM1" s="50"/>
+      <c r="AN1" s="50"/>
+      <c r="AO1" s="50"/>
+      <c r="AP1" s="50"/>
+      <c r="AQ1" s="50"/>
+      <c r="AR1" s="50"/>
+      <c r="AS1" s="50"/>
+      <c r="AT1" s="50"/>
+      <c r="AU1" s="50"/>
+      <c r="AV1" s="50"/>
+      <c r="AW1" s="50"/>
+      <c r="AX1" s="50"/>
+      <c r="AY1" s="50"/>
+      <c r="AZ1" s="50"/>
+      <c r="BA1" s="50"/>
+      <c r="BB1" s="50"/>
+      <c r="BC1" s="50"/>
+      <c r="BD1" s="50"/>
+      <c r="BE1" s="50"/>
+      <c r="BF1" s="50"/>
+    </row>
+    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="24">
+        <v>4</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="G2" s="53" t="s">
+        <v>260</v>
+      </c>
+      <c r="H2" s="53">
+        <v>50</v>
+      </c>
+      <c r="I2" s="52" t="str">
+        <f>_xlfn.CONCAT(D2:H2)</f>
+        <v>000000c350</v>
+      </c>
+      <c r="J2" s="29">
+        <f>HEX2DEC(I2)</f>
+        <v>50000</v>
+      </c>
+      <c r="K2" s="36">
+        <f>J2/1000</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" s="24">
+        <v>4</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E3" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="F3" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="G3" s="53" t="s">
+        <v>233</v>
+      </c>
+      <c r="H3" s="53" t="s">
+        <v>275</v>
+      </c>
+      <c r="I3" s="52" t="str">
+        <f t="shared" ref="I3:I13" si="0">_xlfn.CONCAT(D3:H3)</f>
+        <v>00000007d0</v>
+      </c>
+      <c r="J3" s="29">
+        <f t="shared" ref="J3:J13" si="1">HEX2DEC(I3)</f>
+        <v>2000</v>
+      </c>
+      <c r="K3" s="36">
+        <f>J3/1000</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C4" s="24">
+        <v>4</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="F4" s="53" t="s">
+        <v>226</v>
+      </c>
+      <c r="G4" s="53">
+        <v>86</v>
+      </c>
+      <c r="H4" s="53" t="s">
+        <v>263</v>
+      </c>
+      <c r="I4" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>00000186a0</v>
+      </c>
+      <c r="J4" s="29">
+        <f t="shared" si="1"/>
+        <v>100000</v>
+      </c>
+      <c r="K4" s="36">
+        <f>J4/1000</f>
+        <v>100</v>
+      </c>
+      <c r="M4" s="54" t="s">
+        <v>273</v>
+      </c>
+      <c r="N4" s="54"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="54"/>
+      <c r="R4" s="54"/>
+      <c r="S4" s="54"/>
+      <c r="T4" s="54"/>
+      <c r="U4" s="54"/>
+      <c r="V4" s="54"/>
+      <c r="W4" s="54"/>
+      <c r="X4" s="54"/>
+      <c r="Y4" s="54"/>
+      <c r="Z4" s="54"/>
+      <c r="AA4" s="54"/>
+      <c r="AB4" s="54"/>
+      <c r="AC4" s="54"/>
+      <c r="AD4" s="54"/>
+      <c r="AE4" s="54"/>
+      <c r="AF4" s="54"/>
+      <c r="AG4" s="54"/>
+      <c r="AH4" s="54"/>
+      <c r="AI4" s="54"/>
+      <c r="AJ4" s="54"/>
+      <c r="AK4" s="54"/>
+      <c r="AL4" s="54"/>
+      <c r="AM4" s="54"/>
+      <c r="AN4" s="54"/>
+      <c r="AO4" s="54"/>
+      <c r="AP4" s="54"/>
+      <c r="AQ4" s="54"/>
+      <c r="AR4" s="54"/>
+      <c r="AS4" s="54"/>
+      <c r="AT4" s="54"/>
+      <c r="AU4" s="54"/>
+      <c r="AV4" s="54"/>
+      <c r="AW4" s="54"/>
+      <c r="AX4" s="54"/>
+      <c r="AY4" s="54"/>
+      <c r="AZ4" s="54"/>
+      <c r="BA4" s="54"/>
+      <c r="BB4" s="54"/>
+      <c r="BC4" s="54"/>
+      <c r="BD4" s="54"/>
+      <c r="BE4" s="54"/>
+      <c r="BF4" s="54"/>
+      <c r="BG4" s="54"/>
+    </row>
+    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5" s="24">
+        <v>2</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E5" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="F5" s="53" t="s">
+        <v>264</v>
+      </c>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>0000fa</v>
+      </c>
+      <c r="J5" s="29">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="K5" s="37">
+        <f>INT(J5/10)</f>
+        <v>25</v>
+      </c>
+      <c r="M5" s="55" t="s">
+        <v>258</v>
+      </c>
+      <c r="N5" s="55">
+        <v>55</v>
+      </c>
+      <c r="O5" s="55" t="s">
+        <v>226</v>
+      </c>
+      <c r="P5" s="55" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q5" s="56" t="s">
+        <v>208</v>
+      </c>
+      <c r="R5" s="56" t="s">
+        <v>208</v>
+      </c>
+      <c r="S5" s="57" t="s">
+        <v>260</v>
+      </c>
+      <c r="T5" s="57">
+        <v>50</v>
+      </c>
+      <c r="U5" s="57" t="s">
+        <v>208</v>
+      </c>
+      <c r="V5" s="57" t="s">
+        <v>208</v>
+      </c>
+      <c r="W5" s="57" t="s">
+        <v>261</v>
+      </c>
+      <c r="X5" s="57" t="s">
+        <v>262</v>
+      </c>
+      <c r="Y5" s="57" t="s">
+        <v>208</v>
+      </c>
+      <c r="Z5" s="57" t="s">
+        <v>226</v>
+      </c>
+      <c r="AA5" s="57">
+        <v>86</v>
+      </c>
+      <c r="AB5" s="57" t="s">
+        <v>263</v>
+      </c>
+      <c r="AC5" s="57" t="s">
+        <v>208</v>
+      </c>
+      <c r="AD5" s="57" t="s">
+        <v>264</v>
+      </c>
+      <c r="AE5" s="57" t="s">
+        <v>208</v>
+      </c>
+      <c r="AF5" s="57">
+        <v>32</v>
+      </c>
+      <c r="AG5" s="57" t="s">
+        <v>208</v>
+      </c>
+      <c r="AH5" s="57">
+        <v>80</v>
+      </c>
+      <c r="AI5" s="57" t="s">
+        <v>265</v>
+      </c>
+      <c r="AJ5" s="57" t="s">
+        <v>266</v>
+      </c>
+      <c r="AK5" s="57" t="s">
+        <v>267</v>
+      </c>
+      <c r="AL5" s="57" t="s">
+        <v>268</v>
+      </c>
+      <c r="AM5" s="57" t="s">
+        <v>265</v>
+      </c>
+      <c r="AN5" s="57" t="s">
+        <v>266</v>
+      </c>
+      <c r="AO5" s="57" t="s">
+        <v>189</v>
+      </c>
+      <c r="AP5" s="57">
+        <v>10</v>
+      </c>
+      <c r="AQ5" s="57" t="s">
+        <v>265</v>
+      </c>
+      <c r="AR5" s="57" t="s">
+        <v>266</v>
+      </c>
+      <c r="AS5" s="57" t="s">
+        <v>269</v>
+      </c>
+      <c r="AT5" s="57" t="s">
+        <v>208</v>
+      </c>
+      <c r="AU5" s="57" t="s">
+        <v>265</v>
+      </c>
+      <c r="AV5" s="57" t="s">
+        <v>266</v>
+      </c>
+      <c r="AW5" s="57" t="s">
+        <v>270</v>
+      </c>
+      <c r="AX5" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="AY5" s="57" t="s">
+        <v>208</v>
+      </c>
+      <c r="AZ5" s="57" t="s">
+        <v>271</v>
+      </c>
+      <c r="BA5" s="57" t="s">
+        <v>272</v>
+      </c>
+      <c r="BB5" s="57">
+        <v>10</v>
+      </c>
+      <c r="BC5" s="57" t="s">
+        <v>208</v>
+      </c>
+      <c r="BD5" s="57" t="s">
+        <v>271</v>
+      </c>
+      <c r="BE5" s="57">
+        <v>42</v>
+      </c>
+      <c r="BF5" s="57">
+        <v>40</v>
+      </c>
+      <c r="BG5" s="58">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C6" s="24">
+        <v>2</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E6" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="F6" s="53">
+        <v>32</v>
+      </c>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>000032</v>
+      </c>
+      <c r="J6" s="29">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="K6" s="37">
+        <f>INT(J6/10)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" s="24">
+        <v>2</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E7" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="F7" s="53">
+        <v>80</v>
+      </c>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>000080</v>
+      </c>
+      <c r="J7" s="29">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="K7" s="37">
+        <f>INT(J7)</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C8" s="24">
+        <v>4</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E8" s="53" t="s">
+        <v>265</v>
+      </c>
+      <c r="F8" s="53" t="s">
+        <v>266</v>
+      </c>
+      <c r="G8" s="53" t="s">
+        <v>267</v>
+      </c>
+      <c r="H8" s="53" t="s">
+        <v>268</v>
+      </c>
+      <c r="I8" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>003b9aa2f0</v>
+      </c>
+      <c r="J8" s="29">
+        <f t="shared" si="1"/>
+        <v>999990000</v>
+      </c>
+      <c r="K8" s="37">
+        <f>INT(J8-1000000000)</f>
+        <v>-10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C9" s="24">
+        <v>4</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E9" s="53" t="s">
+        <v>265</v>
+      </c>
+      <c r="F9" s="53" t="s">
+        <v>266</v>
+      </c>
+      <c r="G9" s="53" t="s">
+        <v>189</v>
+      </c>
+      <c r="H9" s="53">
+        <v>10</v>
+      </c>
+      <c r="I9" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>003b9af110</v>
+      </c>
+      <c r="J9" s="29">
+        <f t="shared" si="1"/>
+        <v>1000010000</v>
+      </c>
+      <c r="K9" s="37">
+        <f>INT(J9-1000000000)</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C10" s="24">
+        <v>4</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E10" s="53" t="s">
+        <v>265</v>
+      </c>
+      <c r="F10" s="53" t="s">
+        <v>266</v>
+      </c>
+      <c r="G10" s="53" t="s">
+        <v>269</v>
+      </c>
+      <c r="H10" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="I10" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>003b9aca00</v>
+      </c>
+      <c r="J10" s="29">
+        <f t="shared" si="1"/>
+        <v>1000000000</v>
+      </c>
+      <c r="K10" s="37">
+        <f>INT(J10-1000000000)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C11" s="24">
+        <v>4</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E11" s="53" t="s">
+        <v>265</v>
+      </c>
+      <c r="F11" s="53" t="s">
+        <v>266</v>
+      </c>
+      <c r="G11" s="53" t="s">
+        <v>270</v>
+      </c>
+      <c r="H11" s="53" t="s">
+        <v>203</v>
+      </c>
+      <c r="I11" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>003b9ad9ff</v>
+      </c>
+      <c r="J11" s="29">
+        <f t="shared" si="1"/>
+        <v>1000004095</v>
+      </c>
+      <c r="K11" s="37">
+        <f>INT(J11-1000000000)</f>
+        <v>4095</v>
+      </c>
+    </row>
+    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C12" s="24">
+        <v>4</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E12" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="F12" s="53" t="s">
+        <v>271</v>
+      </c>
+      <c r="G12" s="53" t="s">
+        <v>272</v>
+      </c>
+      <c r="H12" s="53">
+        <v>10</v>
+      </c>
+      <c r="I12" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>00000f4a10</v>
+      </c>
+      <c r="J12" s="29">
+        <f t="shared" si="1"/>
+        <v>1002000</v>
+      </c>
+      <c r="K12" s="38">
+        <f>(J12-1000000)/1000</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C13" s="24">
+        <v>4</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E13" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="F13" s="53" t="s">
+        <v>271</v>
+      </c>
+      <c r="G13" s="53">
+        <v>42</v>
+      </c>
+      <c r="H13" s="53">
+        <v>40</v>
+      </c>
+      <c r="I13" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>00000f4240</v>
+      </c>
+      <c r="J13" s="29">
+        <f t="shared" si="1"/>
+        <v>1000000</v>
+      </c>
+      <c r="K13" s="36">
+        <f>(J13-1000000)/1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B14" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="C14" s="3">
+        <f>SUM(C2:C13)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:59" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="H18" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="I18" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="J18" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="K18" s="35" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="19" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>1</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C19" s="24">
+        <v>4</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="G19" s="53" t="s">
+        <v>260</v>
+      </c>
+      <c r="H19" s="53">
+        <v>50</v>
+      </c>
+      <c r="I19" s="52" t="str">
+        <f>_xlfn.CONCAT(D19:H19)</f>
+        <v>000000c350</v>
+      </c>
+      <c r="J19" s="29">
+        <f>HEX2DEC(I19)</f>
+        <v>50000</v>
+      </c>
+      <c r="K19" s="36">
+        <f>J19/1000</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>2</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C20" s="24">
+        <v>4</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E20" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="F20" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="G20" s="53" t="s">
+        <v>261</v>
+      </c>
+      <c r="H20" s="53" t="s">
+        <v>262</v>
+      </c>
+      <c r="I20" s="52" t="str">
+        <f t="shared" ref="I20:I30" si="2">_xlfn.CONCAT(D20:H20)</f>
+        <v>0000000bb8</v>
+      </c>
+      <c r="J20" s="29">
+        <f t="shared" ref="J20:J30" si="3">HEX2DEC(I20)</f>
+        <v>3000</v>
+      </c>
+      <c r="K20" s="36">
+        <f>J20/1000</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>3</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C21" s="24">
+        <v>4</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E21" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="F21" s="53" t="s">
+        <v>226</v>
+      </c>
+      <c r="G21" s="53">
+        <v>86</v>
+      </c>
+      <c r="H21" s="53" t="s">
+        <v>263</v>
+      </c>
+      <c r="I21" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>00000186a0</v>
+      </c>
+      <c r="J21" s="29">
+        <f t="shared" si="3"/>
+        <v>100000</v>
+      </c>
+      <c r="K21" s="36">
+        <f>J21/1000</f>
+        <v>100</v>
+      </c>
+      <c r="M21" s="54" t="s">
+        <v>273</v>
+      </c>
+      <c r="N21" s="54"/>
+      <c r="O21" s="54"/>
+      <c r="P21" s="54"/>
+      <c r="Q21" s="54"/>
+      <c r="R21" s="54"/>
+      <c r="S21" s="54"/>
+      <c r="T21" s="54"/>
+      <c r="U21" s="54"/>
+      <c r="V21" s="54"/>
+      <c r="W21" s="54"/>
+      <c r="X21" s="54"/>
+      <c r="Y21" s="54"/>
+      <c r="Z21" s="54"/>
+      <c r="AA21" s="54"/>
+      <c r="AB21" s="54"/>
+      <c r="AC21" s="54"/>
+      <c r="AD21" s="54"/>
+      <c r="AE21" s="54"/>
+      <c r="AF21" s="54"/>
+      <c r="AG21" s="54"/>
+      <c r="AH21" s="54"/>
+      <c r="AI21" s="54"/>
+      <c r="AJ21" s="54"/>
+      <c r="AK21" s="54"/>
+      <c r="AL21" s="54"/>
+      <c r="AM21" s="54"/>
+      <c r="AN21" s="54"/>
+      <c r="AO21" s="54"/>
+      <c r="AP21" s="54"/>
+      <c r="AQ21" s="54"/>
+      <c r="AR21" s="54"/>
+      <c r="AS21" s="54"/>
+      <c r="AT21" s="54"/>
+      <c r="AU21" s="54"/>
+      <c r="AV21" s="54"/>
+      <c r="AW21" s="54"/>
+      <c r="AX21" s="54"/>
+      <c r="AY21" s="54"/>
+      <c r="AZ21" s="54"/>
+      <c r="BA21" s="54"/>
+      <c r="BB21" s="54"/>
+      <c r="BC21" s="54"/>
+      <c r="BD21" s="54"/>
+      <c r="BE21" s="54"/>
+      <c r="BF21" s="54"/>
+      <c r="BG21" s="54"/>
+    </row>
+    <row r="22" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>4</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C22" s="24">
+        <v>2</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E22" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="F22" s="53" t="s">
+        <v>264</v>
+      </c>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>0000fa</v>
+      </c>
+      <c r="J22" s="29">
+        <f t="shared" si="3"/>
+        <v>250</v>
+      </c>
+      <c r="K22" s="37">
+        <f>INT(J22/10)</f>
+        <v>25</v>
+      </c>
+      <c r="M22" s="55" t="s">
+        <v>258</v>
+      </c>
+      <c r="N22" s="55">
+        <v>55</v>
+      </c>
+      <c r="O22" s="55" t="s">
+        <v>212</v>
+      </c>
+      <c r="P22" s="55" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q22" s="56" t="s">
+        <v>208</v>
+      </c>
+      <c r="R22" s="56" t="s">
+        <v>208</v>
+      </c>
+      <c r="S22" s="57" t="s">
+        <v>260</v>
+      </c>
+      <c r="T22" s="57">
+        <v>50</v>
+      </c>
+      <c r="U22" s="57" t="s">
+        <v>208</v>
+      </c>
+      <c r="V22" s="57" t="s">
+        <v>208</v>
+      </c>
+      <c r="W22" s="57" t="s">
+        <v>261</v>
+      </c>
+      <c r="X22" s="57" t="s">
+        <v>262</v>
+      </c>
+      <c r="Y22" s="57" t="s">
+        <v>208</v>
+      </c>
+      <c r="Z22" s="57" t="s">
+        <v>226</v>
+      </c>
+      <c r="AA22" s="57">
+        <v>86</v>
+      </c>
+      <c r="AB22" s="57" t="s">
+        <v>263</v>
+      </c>
+      <c r="AC22" s="57" t="s">
+        <v>208</v>
+      </c>
+      <c r="AD22" s="57" t="s">
+        <v>264</v>
+      </c>
+      <c r="AE22" s="57" t="s">
+        <v>208</v>
+      </c>
+      <c r="AF22" s="57">
+        <v>32</v>
+      </c>
+      <c r="AG22" s="57" t="s">
+        <v>208</v>
+      </c>
+      <c r="AH22" s="57">
+        <v>80</v>
+      </c>
+      <c r="AI22" s="57" t="s">
+        <v>265</v>
+      </c>
+      <c r="AJ22" s="57" t="s">
+        <v>266</v>
+      </c>
+      <c r="AK22" s="57" t="s">
+        <v>267</v>
+      </c>
+      <c r="AL22" s="57" t="s">
+        <v>268</v>
+      </c>
+      <c r="AM22" s="57" t="s">
+        <v>265</v>
+      </c>
+      <c r="AN22" s="57" t="s">
+        <v>266</v>
+      </c>
+      <c r="AO22" s="57" t="s">
+        <v>189</v>
+      </c>
+      <c r="AP22" s="57">
+        <v>10</v>
+      </c>
+      <c r="AQ22" s="57" t="s">
+        <v>265</v>
+      </c>
+      <c r="AR22" s="57" t="s">
+        <v>266</v>
+      </c>
+      <c r="AS22" s="57" t="s">
+        <v>269</v>
+      </c>
+      <c r="AT22" s="57" t="s">
+        <v>208</v>
+      </c>
+      <c r="AU22" s="57" t="s">
+        <v>265</v>
+      </c>
+      <c r="AV22" s="57" t="s">
+        <v>266</v>
+      </c>
+      <c r="AW22" s="57" t="s">
+        <v>270</v>
+      </c>
+      <c r="AX22" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="AY22" s="57" t="s">
+        <v>208</v>
+      </c>
+      <c r="AZ22" s="57" t="s">
+        <v>271</v>
+      </c>
+      <c r="BA22" s="57" t="s">
+        <v>272</v>
+      </c>
+      <c r="BB22" s="57">
+        <v>10</v>
+      </c>
+      <c r="BC22" s="57" t="s">
+        <v>208</v>
+      </c>
+      <c r="BD22" s="57" t="s">
+        <v>271</v>
+      </c>
+      <c r="BE22" s="57">
+        <v>42</v>
+      </c>
+      <c r="BF22" s="57">
+        <v>40</v>
+      </c>
+      <c r="BG22" s="58" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="23" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>5</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C23" s="24">
+        <v>2</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E23" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="F23" s="53">
+        <v>32</v>
+      </c>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>000032</v>
+      </c>
+      <c r="J23" s="29">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="K23" s="37">
+        <f>INT(J23/10)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>6</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C24" s="24">
+        <v>2</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E24" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="F24" s="53">
+        <v>80</v>
+      </c>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>000080</v>
+      </c>
+      <c r="J24" s="29">
+        <f t="shared" si="3"/>
+        <v>128</v>
+      </c>
+      <c r="K24" s="37">
+        <f>INT(J24)</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>7</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C25" s="24">
+        <v>4</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E25" s="53" t="s">
+        <v>265</v>
+      </c>
+      <c r="F25" s="53" t="s">
+        <v>266</v>
+      </c>
+      <c r="G25" s="53" t="s">
+        <v>267</v>
+      </c>
+      <c r="H25" s="53" t="s">
+        <v>268</v>
+      </c>
+      <c r="I25" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>003b9aa2f0</v>
+      </c>
+      <c r="J25" s="29">
+        <f t="shared" si="3"/>
+        <v>999990000</v>
+      </c>
+      <c r="K25" s="37">
+        <f>INT(J25-1000000000)</f>
+        <v>-10000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>8</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C26" s="24">
+        <v>4</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E26" s="53" t="s">
+        <v>265</v>
+      </c>
+      <c r="F26" s="53" t="s">
+        <v>266</v>
+      </c>
+      <c r="G26" s="53" t="s">
+        <v>189</v>
+      </c>
+      <c r="H26" s="53">
+        <v>10</v>
+      </c>
+      <c r="I26" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>003b9af110</v>
+      </c>
+      <c r="J26" s="29">
+        <f t="shared" si="3"/>
+        <v>1000010000</v>
+      </c>
+      <c r="K26" s="37">
+        <f>INT(J26-1000000000)</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>9</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C27" s="24">
+        <v>4</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E27" s="53" t="s">
+        <v>265</v>
+      </c>
+      <c r="F27" s="53" t="s">
+        <v>266</v>
+      </c>
+      <c r="G27" s="53" t="s">
+        <v>269</v>
+      </c>
+      <c r="H27" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="I27" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>003b9aca00</v>
+      </c>
+      <c r="J27" s="29">
+        <f t="shared" si="3"/>
+        <v>1000000000</v>
+      </c>
+      <c r="K27" s="37">
+        <f>INT(J27-1000000000)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>10</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C28" s="24">
+        <v>4</v>
+      </c>
+      <c r="D28" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E28" s="53" t="s">
+        <v>265</v>
+      </c>
+      <c r="F28" s="53" t="s">
+        <v>266</v>
+      </c>
+      <c r="G28" s="53" t="s">
+        <v>270</v>
+      </c>
+      <c r="H28" s="53" t="s">
+        <v>203</v>
+      </c>
+      <c r="I28" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>003b9ad9ff</v>
+      </c>
+      <c r="J28" s="29">
+        <f t="shared" si="3"/>
+        <v>1000004095</v>
+      </c>
+      <c r="K28" s="37">
+        <f>INT(J28-1000000000)</f>
+        <v>4095</v>
+      </c>
+    </row>
+    <row r="29" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>11</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C29" s="24">
+        <v>4</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E29" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="F29" s="53" t="s">
+        <v>271</v>
+      </c>
+      <c r="G29" s="53" t="s">
+        <v>272</v>
+      </c>
+      <c r="H29" s="53">
+        <v>10</v>
+      </c>
+      <c r="I29" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>00000f4a10</v>
+      </c>
+      <c r="J29" s="29">
+        <f t="shared" si="3"/>
+        <v>1002000</v>
+      </c>
+      <c r="K29" s="38">
+        <f>(J29-1000000)/1000</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>12</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C30" s="24">
+        <v>4</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E30" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="F30" s="53" t="s">
+        <v>271</v>
+      </c>
+      <c r="G30" s="53">
+        <v>42</v>
+      </c>
+      <c r="H30" s="53">
+        <v>40</v>
+      </c>
+      <c r="I30" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>00000f4240</v>
+      </c>
+      <c r="J30" s="29">
+        <f t="shared" si="3"/>
+        <v>1000000</v>
+      </c>
+      <c r="K30" s="36">
+        <f>(J30-1000000)/1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B31" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="C31" s="3">
+        <f>SUM(C19:C30)</f>
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="M4:BG4"/>
+    <mergeCell ref="M21:BG21"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>